<commit_message>
Remove ts duration input from SysSettings.xlsx
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFB509F-FB45-445E-8C5A-2FFD88E73A96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B5AC97-637E-499E-BB81-1240F2CC9807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="853" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -305,18 +305,12 @@
     <t>~ActivePDef</t>
   </si>
   <si>
-    <t>YRFR</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>Timeslice List</t>
-  </si>
-  <si>
     <t>IE</t>
   </si>
   <si>
@@ -381,54 +375,6 @@
   </si>
   <si>
     <t>Commodity_Unit</t>
-  </si>
-  <si>
-    <t>Source: UKTM</t>
-  </si>
-  <si>
-    <t>Period</t>
-  </si>
-  <si>
-    <t>Period code</t>
-  </si>
-  <si>
-    <t>Start time</t>
-  </si>
-  <si>
-    <t>End time</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Evening peak</t>
-  </si>
-  <si>
-    <t>Late evening</t>
-  </si>
-  <si>
-    <t>Night</t>
-  </si>
-  <si>
-    <t>17.00</t>
-  </si>
-  <si>
-    <t>20.00</t>
-  </si>
-  <si>
-    <t>00.00</t>
-  </si>
-  <si>
-    <t>07.00</t>
-  </si>
-  <si>
-    <t>Season length</t>
-  </si>
-  <si>
-    <t>1/4 of the year</t>
   </si>
   <si>
     <t>DumVarforUC</t>
@@ -684,7 +630,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -738,11 +684,6 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -829,7 +770,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,14 +825,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1008,116 +943,44 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1129,72 +992,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1207,22 +1029,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1254,7 +1075,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>23813</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1500,7 +1321,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>36210</xdr:rowOff>
     </xdr:to>
@@ -3438,643 +3259,642 @@
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" style="71" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="71" customWidth="1"/>
-    <col min="3" max="3" width="3.1328125" style="71" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.53125" style="71" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.46484375" style="71" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.9296875" style="71" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.73046875" style="71" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.86328125" style="71" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.46484375" style="71" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.73046875" style="71" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.59765625" style="71" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.06640625" style="71" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="71" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.53125" style="71" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.19921875" style="71" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="71" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.06640625" style="71" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.796875" style="71" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.59765625" style="71" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.86328125" style="71" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" style="71" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.9296875" style="71" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.53125" style="71" customWidth="1"/>
-    <col min="25" max="25" width="6.73046875" style="71" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.06640625" style="71" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="6" style="71" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.73046875" style="71" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="71" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.06640625" style="71"/>
+    <col min="1" max="1" width="12.140625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="52" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" style="52" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5" style="52" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="52" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="6" style="52" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9" style="52"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="14.25" x14ac:dyDescent="0.35">
-      <c r="C3" s="72" t="str" cm="1">
+    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="C3" s="53" t="str" cm="1">
         <f t="array" ref="C3">IF(INDEX(C5:C7,$A$4)&lt;&gt;0,INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
       </c>
-      <c r="D3" s="72" t="str" cm="1">
+      <c r="D3" s="53" t="str" cm="1">
         <f t="array" ref="D3">IF(INDEX(D5:D7,$A$4)&lt;&gt;0,INDEX(D5:D7,$A$4),"")</f>
         <v>National</v>
       </c>
-      <c r="E3" s="72" t="str" cm="1">
+      <c r="E3" s="53" t="str" cm="1">
         <f t="array" ref="E3">IF(INDEX(E5:E7,$A$4)&lt;&gt;0,INDEX(E5:E7,$A$4),"")</f>
         <v>IE-CW</v>
       </c>
-      <c r="F3" s="72" t="str" cm="1">
+      <c r="F3" s="53" t="str" cm="1">
         <f t="array" ref="F3">IF(INDEX(F5:F7,$A$4)&lt;&gt;0,INDEX(F5:F7,$A$4),"")</f>
         <v>IE-D</v>
       </c>
-      <c r="G3" s="72" t="str" cm="1">
+      <c r="G3" s="53" t="str" cm="1">
         <f t="array" ref="G3">IF(INDEX(G5:G7,$A$4)&lt;&gt;0,INDEX(G5:G7,$A$4),"")</f>
         <v>IE-KE</v>
       </c>
-      <c r="H3" s="72" t="str" cm="1">
+      <c r="H3" s="53" t="str" cm="1">
         <f t="array" ref="H3">IF(INDEX(H5:H7,$A$4)&lt;&gt;0,INDEX(H5:H7,$A$4),"")</f>
         <v>IE-KK</v>
       </c>
-      <c r="I3" s="72" t="str" cm="1">
+      <c r="I3" s="53" t="str" cm="1">
         <f t="array" ref="I3">IF(INDEX(I5:I7,$A$4)&lt;&gt;0,INDEX(I5:I7,$A$4),"")</f>
         <v>IE-LS</v>
       </c>
-      <c r="J3" s="72" t="str" cm="1">
+      <c r="J3" s="53" t="str" cm="1">
         <f t="array" ref="J3">IF(INDEX(J5:J7,$A$4)&lt;&gt;0,INDEX(J5:J7,$A$4),"")</f>
         <v>IE-LD</v>
       </c>
-      <c r="K3" s="72" t="str" cm="1">
+      <c r="K3" s="53" t="str" cm="1">
         <f t="array" ref="K3">IF(INDEX(K5:K7,$A$4)&lt;&gt;0,INDEX(K5:K7,$A$4),"")</f>
         <v>IE-LH</v>
       </c>
-      <c r="L3" s="72" t="str" cm="1">
+      <c r="L3" s="53" t="str" cm="1">
         <f t="array" ref="L3">IF(INDEX(L5:L7,$A$4)&lt;&gt;0,INDEX(L5:L7,$A$4),"")</f>
         <v>IE-MH</v>
       </c>
-      <c r="M3" s="72" t="str" cm="1">
+      <c r="M3" s="53" t="str" cm="1">
         <f t="array" ref="M3">IF(INDEX(M5:M7,$A$4)&lt;&gt;0,INDEX(M5:M7,$A$4),"")</f>
         <v>IE-OY</v>
       </c>
-      <c r="N3" s="72" t="str" cm="1">
+      <c r="N3" s="53" t="str" cm="1">
         <f t="array" ref="N3">IF(INDEX(N5:N7,$A$4)&lt;&gt;0,INDEX(N5:N7,$A$4),"")</f>
         <v>IE-WH</v>
       </c>
-      <c r="O3" s="72" t="str" cm="1">
+      <c r="O3" s="53" t="str" cm="1">
         <f t="array" ref="O3">IF(INDEX(O5:O7,$A$4)&lt;&gt;0,INDEX(O5:O7,$A$4),"")</f>
         <v>IE-WX</v>
       </c>
-      <c r="P3" s="72" t="str" cm="1">
+      <c r="P3" s="53" t="str" cm="1">
         <f t="array" ref="P3">IF(INDEX(P5:P7,$A$4)&lt;&gt;0,INDEX(P5:P7,$A$4),"")</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q3" s="72" t="str" cm="1">
+      <c r="Q3" s="53" t="str" cm="1">
         <f t="array" ref="Q3">IF(INDEX(Q5:Q7,$A$4)&lt;&gt;0,INDEX(Q5:Q7,$A$4),"")</f>
         <v>IE-CE</v>
       </c>
-      <c r="R3" s="72" t="str" cm="1">
+      <c r="R3" s="53" t="str" cm="1">
         <f t="array" ref="R3">IF(INDEX(R5:R7,$A$4)&lt;&gt;0,INDEX(R5:R7,$A$4),"")</f>
         <v>IE-CO</v>
       </c>
-      <c r="S3" s="72" t="str" cm="1">
+      <c r="S3" s="53" t="str" cm="1">
         <f t="array" ref="S3">IF(INDEX(S5:S7,$A$4)&lt;&gt;0,INDEX(S5:S7,$A$4),"")</f>
         <v>IE-KY</v>
       </c>
-      <c r="T3" s="72" t="str" cm="1">
+      <c r="T3" s="53" t="str" cm="1">
         <f t="array" ref="T3">IF(INDEX(T5:T7,$A$4)&lt;&gt;0,INDEX(T5:T7,$A$4),"")</f>
         <v>IE-LK</v>
       </c>
-      <c r="U3" s="72" t="str" cm="1">
+      <c r="U3" s="53" t="str" cm="1">
         <f t="array" ref="U3">IF(INDEX(U5:U7,$A$4)&lt;&gt;0,INDEX(U5:U7,$A$4),"")</f>
         <v>IE-TA</v>
       </c>
-      <c r="V3" s="72" t="str" cm="1">
+      <c r="V3" s="53" t="str" cm="1">
         <f t="array" ref="V3">IF(INDEX(V5:V7,$A$4)&lt;&gt;0,INDEX(V5:V7,$A$4),"")</f>
         <v>IE-WD</v>
       </c>
-      <c r="W3" s="72" t="str" cm="1">
+      <c r="W3" s="53" t="str" cm="1">
         <f t="array" ref="W3">IF(INDEX(W5:W7,$A$4)&lt;&gt;0,INDEX(W5:W7,$A$4),"")</f>
         <v>IE-G</v>
       </c>
-      <c r="X3" s="72" t="str" cm="1">
+      <c r="X3" s="53" t="str" cm="1">
         <f t="array" ref="X3">IF(INDEX(X5:X7,$A$4)&lt;&gt;0,INDEX(X5:X7,$A$4),"")</f>
         <v>IE-LM</v>
       </c>
-      <c r="Y3" s="72" t="str" cm="1">
+      <c r="Y3" s="53" t="str" cm="1">
         <f t="array" ref="Y3">IF(INDEX(Y5:Y7,$A$4)&lt;&gt;0,INDEX(Y5:Y7,$A$4),"")</f>
         <v>IE-MO</v>
       </c>
-      <c r="Z3" s="72" t="str" cm="1">
+      <c r="Z3" s="53" t="str" cm="1">
         <f t="array" ref="Z3">IF(INDEX(Z5:Z7,$A$4)&lt;&gt;0,INDEX(Z5:Z7,$A$4),"")</f>
         <v>IE-RN</v>
       </c>
-      <c r="AA3" s="72" t="str" cm="1">
+      <c r="AA3" s="53" t="str" cm="1">
         <f t="array" ref="AA3">IF(INDEX(AA5:AA7,$A$4)&lt;&gt;0,INDEX(AA5:AA7,$A$4),"")</f>
         <v>IE-SO</v>
       </c>
-      <c r="AB3" s="72" t="str" cm="1">
+      <c r="AB3" s="53" t="str" cm="1">
         <f t="array" ref="AB3">IF(INDEX(AB5:AB7,$A$4)&lt;&gt;0,INDEX(AB5:AB7,$A$4),"")</f>
         <v>IE-CN</v>
       </c>
-      <c r="AC3" s="72" t="str" cm="1">
+      <c r="AC3" s="53" t="str" cm="1">
         <f t="array" ref="AC3">IF(INDEX(AC5:AC7,$A$4)&lt;&gt;0,INDEX(AC5:AC7,$A$4),"")</f>
         <v>IE-DL</v>
       </c>
-      <c r="AD3" s="72" t="str" cm="1">
+      <c r="AD3" s="53" t="str" cm="1">
         <f t="array" ref="AD3">IF(INDEX(AD5:AD7,$A$4)&lt;&gt;0,INDEX(AD5:AD7,$A$4),"")</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="73" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71">
+    <row r="4" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="52">
         <v>1</v>
       </c>
-      <c r="B4" s="71"/>
-    </row>
-    <row r="5" spans="1:30" ht="14.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="74" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="74" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="72" t="str">
+      <c r="B4" s="52"/>
+    </row>
+    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="53" t="str">
         <f>A11</f>
         <v>IE-CW</v>
       </c>
-      <c r="F5" s="72" t="str">
+      <c r="F5" s="53" t="str">
         <f>A16</f>
         <v>IE-D</v>
       </c>
-      <c r="G5" s="72" t="str">
+      <c r="G5" s="53" t="str">
         <f>A19</f>
         <v>IE-KE</v>
       </c>
-      <c r="H5" s="72" t="str">
+      <c r="H5" s="53" t="str">
         <f>A20</f>
         <v>IE-KK</v>
       </c>
-      <c r="I5" s="72" t="str">
+      <c r="I5" s="53" t="str">
         <f>A21</f>
         <v>IE-LS</v>
       </c>
-      <c r="J5" s="72" t="str">
+      <c r="J5" s="53" t="str">
         <f>A24</f>
         <v>IE-LD</v>
       </c>
-      <c r="K5" s="72" t="str">
+      <c r="K5" s="53" t="str">
         <f>A25</f>
         <v>IE-LH</v>
       </c>
-      <c r="L5" s="72" t="str">
+      <c r="L5" s="53" t="str">
         <f>A27</f>
         <v>IE-MH</v>
       </c>
-      <c r="M5" s="72" t="str">
+      <c r="M5" s="53" t="str">
         <f>A29</f>
         <v>IE-OY</v>
       </c>
-      <c r="N5" s="72" t="str">
+      <c r="N5" s="53" t="str">
         <f>A34</f>
         <v>IE-WH</v>
       </c>
-      <c r="O5" s="72" t="str">
+      <c r="O5" s="53" t="str">
         <f>A35</f>
         <v>IE-WX</v>
       </c>
-      <c r="P5" s="72" t="str">
+      <c r="P5" s="53" t="str">
         <f>A36</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q5" s="72" t="str">
+      <c r="Q5" s="53" t="str">
         <f>A13</f>
         <v>IE-CE</v>
       </c>
-      <c r="R5" s="72" t="str">
+      <c r="R5" s="53" t="str">
         <f>A14</f>
         <v>IE-CO</v>
       </c>
-      <c r="S5" s="72" t="str">
+      <c r="S5" s="53" t="str">
         <f>A18</f>
         <v>IE-KY</v>
       </c>
-      <c r="T5" s="72" t="str">
+      <c r="T5" s="53" t="str">
         <f>A23</f>
         <v>IE-LK</v>
       </c>
-      <c r="U5" s="72" t="str">
+      <c r="U5" s="53" t="str">
         <f>A32</f>
         <v>IE-TA</v>
       </c>
-      <c r="V5" s="72" t="str">
+      <c r="V5" s="53" t="str">
         <f>A33</f>
         <v>IE-WD</v>
       </c>
-      <c r="W5" s="72" t="str">
+      <c r="W5" s="53" t="str">
         <f>A17</f>
         <v>IE-G</v>
       </c>
-      <c r="X5" s="72" t="str">
+      <c r="X5" s="53" t="str">
         <f>A22</f>
         <v>IE-LM</v>
       </c>
-      <c r="Y5" s="72" t="str">
+      <c r="Y5" s="53" t="str">
         <f>A26</f>
         <v>IE-MO</v>
       </c>
-      <c r="Z5" s="72" t="str">
+      <c r="Z5" s="53" t="str">
         <f>A30</f>
         <v>IE-RN</v>
       </c>
-      <c r="AA5" s="72" t="str">
+      <c r="AA5" s="53" t="str">
         <f>A31</f>
         <v>IE-SO</v>
       </c>
-      <c r="AB5" s="72" t="str">
+      <c r="AB5" s="53" t="str">
         <f>A12</f>
         <v>IE-CN</v>
       </c>
-      <c r="AC5" s="72" t="str">
+      <c r="AC5" s="53" t="str">
         <f>A15</f>
         <v>IE-DL</v>
       </c>
-      <c r="AD5" s="72" t="str">
+      <c r="AD5" s="53" t="str">
         <f>A28</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="14.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="72" t="str">
+    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="53" t="str">
         <f>C5</f>
         <v>IE</v>
       </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="72"/>
-      <c r="U6" s="72"/>
-      <c r="V6" s="72"/>
-      <c r="W6" s="72"/>
-      <c r="X6" s="72"/>
-      <c r="Y6" s="72"/>
-      <c r="Z6" s="72"/>
-      <c r="AA6" s="72"/>
-      <c r="AB6" s="72"/>
-      <c r="AC6" s="72"/>
-      <c r="AD6" s="72"/>
-    </row>
-    <row r="7" spans="1:30" ht="14.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="72" t="str">
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="53"/>
+      <c r="Y6" s="53"/>
+      <c r="Z6" s="53"/>
+      <c r="AA6" s="53"/>
+      <c r="AB6" s="53"/>
+      <c r="AC6" s="53"/>
+      <c r="AD6" s="53"/>
+    </row>
+    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="53" t="str">
         <f t="shared" ref="C7:AC7" si="0">D5</f>
         <v>National</v>
       </c>
-      <c r="D7" s="72" t="str">
+      <c r="D7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-CW</v>
       </c>
-      <c r="E7" s="72" t="str">
+      <c r="E7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-D</v>
       </c>
-      <c r="F7" s="72" t="str">
+      <c r="F7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-KE</v>
       </c>
-      <c r="G7" s="72" t="str">
+      <c r="G7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-KK</v>
       </c>
-      <c r="H7" s="72" t="str">
+      <c r="H7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-LS</v>
       </c>
-      <c r="I7" s="72" t="str">
+      <c r="I7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-LD</v>
       </c>
-      <c r="J7" s="72" t="str">
+      <c r="J7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-LH</v>
       </c>
-      <c r="K7" s="72" t="str">
+      <c r="K7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-MH</v>
       </c>
-      <c r="L7" s="72" t="str">
+      <c r="L7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-OY</v>
       </c>
-      <c r="M7" s="72" t="str">
+      <c r="M7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-WH</v>
       </c>
-      <c r="N7" s="72" t="str">
+      <c r="N7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-WX</v>
       </c>
-      <c r="O7" s="72" t="str">
+      <c r="O7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-WW</v>
       </c>
-      <c r="P7" s="72" t="str">
+      <c r="P7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-CE</v>
       </c>
-      <c r="Q7" s="72" t="str">
+      <c r="Q7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-CO</v>
       </c>
-      <c r="R7" s="72" t="str">
+      <c r="R7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-KY</v>
       </c>
-      <c r="S7" s="72" t="str">
+      <c r="S7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-LK</v>
       </c>
-      <c r="T7" s="72" t="str">
+      <c r="T7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-TA</v>
       </c>
-      <c r="U7" s="72" t="str">
+      <c r="U7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-WD</v>
       </c>
-      <c r="V7" s="72" t="str">
+      <c r="V7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-G</v>
       </c>
-      <c r="W7" s="72" t="str">
+      <c r="W7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-LM</v>
       </c>
-      <c r="X7" s="72" t="str">
+      <c r="X7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-MO</v>
       </c>
-      <c r="Y7" s="72" t="str">
+      <c r="Y7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-RN</v>
       </c>
-      <c r="Z7" s="72" t="str">
+      <c r="Z7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-SO</v>
       </c>
-      <c r="AA7" s="72" t="str">
+      <c r="AA7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-CN</v>
       </c>
-      <c r="AB7" s="72" t="str">
+      <c r="AB7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-DL</v>
       </c>
-      <c r="AC7" s="72" t="str">
+      <c r="AC7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>IE-MN</v>
       </c>
-      <c r="AD7" s="72"/>
-    </row>
-    <row r="10" spans="1:30" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="75" t="s">
+      <c r="AD7" s="53"/>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A15" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A16" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B19" s="58" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A11" s="76" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B20" s="58" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A12" s="77" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B21" s="58" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A13" s="77" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B22" s="58" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A14" s="77" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B23" s="58" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A15" s="77" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B24" s="58" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A16" s="77" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="77" t="s">
+      <c r="B25" s="58" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="77" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="77" t="s">
+      <c r="B26" s="58" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="77" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="77" t="s">
+      <c r="B27" s="58" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="77" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="B19" s="77" t="s">
+      <c r="B28" s="58" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="77" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="B29" s="58" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="77" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="77" t="s">
+      <c r="B30" s="58" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="77" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="77" t="s">
+      <c r="B31" s="58" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="77" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="77" t="s">
+      <c r="B32" s="58" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="77" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="77" t="s">
+      <c r="B33" s="58" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="77" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="77" t="s">
+      <c r="B34" s="58" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="77" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B35" s="58" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="77" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B36" s="58" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="77" t="s">
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="59" t="s">
         <v>136</v>
-      </c>
-      <c r="B28" s="77" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="77" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" s="77" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="77" t="s">
-        <v>140</v>
-      </c>
-      <c r="B30" s="77" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="B31" s="77" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="77" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" s="77" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="77" t="s">
-        <v>146</v>
-      </c>
-      <c r="B33" s="77" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="77" t="s">
-        <v>148</v>
-      </c>
-      <c r="B34" s="77" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="77" t="s">
-        <v>150</v>
-      </c>
-      <c r="B35" s="77" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="77" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="78" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4098,7 +3918,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>23813</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -4116,559 +3936,325 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A3:AJ39"/>
+  <dimension ref="A3:AB39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="5"/>
-    <col min="4" max="4" width="2.1328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.53125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.1328125" style="5"/>
-    <col min="11" max="11" width="9.73046875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1328125" style="5"/>
-    <col min="13" max="13" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="13.265625" style="5" customWidth="1"/>
-    <col min="18" max="16384" width="9.1328125" style="5"/>
+    <col min="1" max="1" width="2.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="4" max="4" width="2.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-    </row>
-    <row r="4" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+    </row>
+    <row r="4" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="58"/>
-      <c r="M4" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="O4" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="P4" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="54" t="str">
+      <c r="B5" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="40" t="str">
         <f>Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="E5" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="5" t="str">
-        <f>$E$5&amp;G5</f>
-        <v>SpD</v>
-      </c>
-      <c r="K5" s="53">
-        <f>Q5/24*0.25</f>
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="M5" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="E5" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="54" t="str">
+      <c r="C6" s="40" t="str">
         <f>Regions!D3</f>
         <v>National</v>
       </c>
-      <c r="E6" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="5" t="str">
-        <f>$E$5&amp;G6</f>
-        <v>SpP</v>
-      </c>
-      <c r="K6" s="53">
-        <f>Q6/24*0.25</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="M6" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="P6" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q6" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="E6" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="54" t="str">
+      <c r="C7" s="40" t="str">
         <f>Regions!E3</f>
         <v>IE-CW</v>
       </c>
-      <c r="E7" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="5" t="str">
-        <f>$E$5&amp;G7</f>
-        <v>SpE</v>
-      </c>
-      <c r="K7" s="53">
-        <f>Q7/24*0.25</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M7" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="N7" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="P7" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q7" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="E7" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="54" t="str">
+      <c r="C8" s="40" t="str">
         <f>Regions!F3</f>
         <v>IE-D</v>
       </c>
-      <c r="E8" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="5" t="str">
-        <f>$E$5&amp;G8</f>
-        <v>SpN</v>
-      </c>
-      <c r="K8" s="53">
-        <f>Q8/24*0.25</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="M8" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="N8" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="O8" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="P8" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="47">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="E8" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="54" t="str">
+      <c r="C9" s="40" t="str">
         <f>Regions!G3</f>
         <v>IE-KE</v>
       </c>
-      <c r="J9" s="5" t="str">
-        <f>$E$6&amp;G5</f>
-        <v>SuD</v>
-      </c>
-      <c r="K9" s="53">
-        <f>K5</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="54" t="str">
+      <c r="C10" s="40" t="str">
         <f>Regions!H3</f>
         <v>IE-KK</v>
       </c>
-      <c r="J10" s="5" t="str">
-        <f t="shared" ref="J10:J12" si="0">$E$6&amp;G6</f>
-        <v>SuP</v>
-      </c>
-      <c r="K10" s="53">
-        <f>K6</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" s="43" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="54" t="str">
+      <c r="C11" s="40" t="str">
         <f>Regions!I3</f>
         <v>IE-LS</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="J11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SuE</v>
-      </c>
-      <c r="K11" s="53">
-        <f>K7</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="E11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="54" t="str">
+      <c r="C12" s="40" t="str">
         <f>Regions!J3</f>
         <v>IE-LD</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="J12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>SuN</v>
-      </c>
-      <c r="K12" s="53">
-        <f>K8</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="E12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="54" t="str">
+      <c r="C13" s="40" t="str">
         <f>Regions!K3</f>
         <v>IE-LH</v>
       </c>
       <c r="E13" s="33"/>
-      <c r="J13" s="5" t="str">
-        <f>$E$7&amp;G5</f>
-        <v>AuD</v>
-      </c>
-      <c r="K13" s="53">
-        <f>K5</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="54" t="str">
+      <c r="C14" s="40" t="str">
         <f>Regions!L3</f>
         <v>IE-MH</v>
       </c>
       <c r="E14" s="33"/>
-      <c r="J14" s="5" t="str">
-        <f t="shared" ref="J14:J16" si="1">$E$7&amp;G6</f>
-        <v>AuP</v>
-      </c>
-      <c r="K14" s="53">
-        <f>K6</f>
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="54" t="str">
+      <c r="C15" s="40" t="str">
         <f>Regions!M3</f>
         <v>IE-OY</v>
       </c>
       <c r="E15" s="33"/>
-      <c r="J15" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AuE</v>
-      </c>
-      <c r="K15" s="53">
-        <f>K7</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="54" t="str">
+      <c r="C16" s="40" t="str">
         <f>Regions!N3</f>
         <v>IE-WH</v>
       </c>
       <c r="E16" s="33"/>
-      <c r="J16" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>AuN</v>
-      </c>
-      <c r="K16" s="53">
-        <f>K8</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="54" t="str">
+      <c r="C17" s="40" t="str">
         <f>Regions!O3</f>
         <v>IE-WX</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="J17" s="5" t="str">
-        <f>$E$8&amp;G5</f>
-        <v>WiD</v>
-      </c>
-      <c r="K17" s="53">
-        <f>K5</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="E17" s="39"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="54" t="str">
+      <c r="C18" s="40" t="str">
         <f>Regions!P3</f>
         <v>IE-WW</v>
       </c>
-      <c r="J18" s="5" t="str">
-        <f t="shared" ref="J18:J20" si="2">$E$8&amp;G6</f>
-        <v>WiP</v>
-      </c>
-      <c r="K18" s="53">
-        <f>K6</f>
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="54" t="str">
+      <c r="C19" s="40" t="str">
         <f>Regions!Q3</f>
         <v>IE-CE</v>
       </c>
-      <c r="J19" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>WiE</v>
-      </c>
-      <c r="K19" s="53">
-        <f>K7</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
-      <c r="C20" s="54" t="str">
+      <c r="C20" s="40" t="str">
         <f>Regions!R3</f>
         <v>IE-CO</v>
       </c>
-      <c r="J20" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>WiN</v>
-      </c>
-      <c r="K20" s="53">
-        <f>K8</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="C21" s="54" t="str">
+      <c r="C21" s="40" t="str">
         <f>Regions!S3</f>
         <v>IE-KY</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K21" s="53"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-      <c r="C22" s="54" t="str">
+      <c r="C22" s="40" t="str">
         <f>Regions!T3</f>
         <v>IE-LK</v>
       </c>
-      <c r="K22" s="53"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
-      <c r="C23" s="54" t="str">
+      <c r="C23" s="40" t="str">
         <f>Regions!U3</f>
         <v>IE-TA</v>
       </c>
-      <c r="K23" s="53"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
-      <c r="C24" s="54" t="str">
+      <c r="C24" s="40" t="str">
         <f>Regions!V3</f>
         <v>IE-WD</v>
       </c>
-      <c r="K24" s="53"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
-      <c r="C25" s="54" t="str">
+      <c r="C25" s="40" t="str">
         <f>Regions!W3</f>
         <v>IE-G</v>
       </c>
-      <c r="K25" s="53"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
-      <c r="C26" s="54" t="str">
+      <c r="C26" s="40" t="str">
         <f>Regions!X3</f>
         <v>IE-LM</v>
       </c>
-      <c r="K26" s="53"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-      <c r="C27" s="54" t="str">
+      <c r="C27" s="40" t="str">
         <f>Regions!Y3</f>
         <v>IE-MO</v>
       </c>
-      <c r="K27" s="53"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
-      <c r="C28" s="54" t="str">
+      <c r="C28" s="40" t="str">
         <f>Regions!Z3</f>
         <v>IE-RN</v>
       </c>
-      <c r="K28" s="53"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
-      <c r="C29" s="54" t="str">
+      <c r="C29" s="40" t="str">
         <f>Regions!AA3</f>
         <v>IE-SO</v>
       </c>
-      <c r="K29" s="53"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
-      <c r="C30" s="54" t="str">
+      <c r="C30" s="40" t="str">
         <f>Regions!AB3</f>
         <v>IE-CN</v>
       </c>
-      <c r="K30" s="53"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
-      <c r="C31" s="54" t="str">
+      <c r="C31" s="40" t="str">
         <f>Regions!AC3</f>
         <v>IE-DL</v>
       </c>
-      <c r="K31" s="53"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
-      <c r="C32" s="54" t="str">
+      <c r="C32" s="40" t="str">
         <f>Regions!AD3</f>
         <v>IE-MN</v>
       </c>
-      <c r="K32" s="53"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="K33" s="53"/>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
-      <c r="AE34" s="54"/>
-      <c r="AF34" s="54"/>
-      <c r="AG34" s="54"/>
-      <c r="AH34" s="54"/>
-      <c r="AI34" s="54"/>
-      <c r="AJ34" s="54"/>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="W34" s="40"/>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="40"/>
+      <c r="AA34" s="40"/>
+      <c r="AB34" s="40"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
     </row>
   </sheetData>
@@ -4689,159 +4275,159 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" customWidth="1"/>
-    <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B3" s="40" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B7" s="40" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B11" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B12" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="66" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="41">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="37">
         <v>1</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B14" s="41">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="37">
         <v>4</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="41">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="37">
         <v>5</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B16" s="41">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="37">
         <v>5</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="41">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="37">
         <v>5</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="41">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="37">
         <v>5</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="41">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="37">
         <v>5</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="41">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="37">
         <v>5</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="41">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="37">
         <v>5</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="41">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="37">
         <v>5</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="41">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="37">
         <v>5</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="41">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="37">
         <v>5</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="41"/>
-      <c r="C25" s="41">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="37"/>
+      <c r="C26" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="41"/>
-      <c r="C27" s="41">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="37"/>
+      <c r="C27" s="37">
         <v>5</v>
       </c>
     </row>
@@ -4862,17 +4448,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="52.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
@@ -4880,43 +4466,43 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" s="63" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="64" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="45">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="41" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B9" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="41">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="37">
         <v>0</v>
       </c>
     </row>
@@ -4934,27 +4520,27 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.1328125" style="5"/>
-    <col min="3" max="3" width="13.1328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1328125" style="5"/>
-    <col min="6" max="6" width="10.73046875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.46484375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.1328125" style="5"/>
-    <col min="12" max="12" width="9.265625" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.1328125" style="5"/>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="5"/>
+    <col min="6" max="6" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="5"/>
+    <col min="12" max="12" width="9.28515625" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -4971,7 +4557,7 @@
       <c r="N2"/>
       <c r="O2" s="6"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -4989,7 +4575,7 @@
       <c r="O3" s="8"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -5007,7 +4593,7 @@
       <c r="O4" s="8"/>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -5025,7 +4611,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="9"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -5043,7 +4629,7 @@
       <c r="O6" s="8"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -5061,7 +4647,7 @@
       <c r="O7" s="8"/>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -5079,7 +4665,7 @@
       <c r="O8" s="8"/>
       <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -5097,7 +4683,7 @@
       <c r="O9" s="8"/>
       <c r="P9" s="9"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -5115,7 +4701,7 @@
       <c r="O10" s="8"/>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -5133,7 +4719,7 @@
       <c r="O11" s="8"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -5151,9 +4737,9 @@
       <c r="O12" s="8"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -5170,7 +4756,7 @@
       <c r="O13" s="8"/>
       <c r="P13" s="9"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>0</v>
       </c>
@@ -5190,7 +4776,7 @@
       <c r="O14" s="8"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
@@ -5210,10 +4796,10 @@
         <v>2</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>20</v>
@@ -5240,7 +4826,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
@@ -5266,7 +4852,7 @@
       <c r="O16" s="8"/>
       <c r="P16" s="9"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
@@ -5292,7 +4878,7 @@
       <c r="O17" s="8"/>
       <c r="P17" s="9"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -5310,7 +4896,7 @@
       <c r="O18" s="8"/>
       <c r="P18" s="9"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -5328,7 +4914,7 @@
       <c r="O19" s="8"/>
       <c r="P19" s="9"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -5346,7 +4932,7 @@
       <c r="O20" s="8"/>
       <c r="P20" s="9"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -5364,13 +4950,13 @@
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="65"/>
+      <c r="F22" s="46"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -5382,7 +4968,7 @@
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -5400,7 +4986,7 @@
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -5430,40 +5016,40 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="B1:G50"/>
+  <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="25"/>
-    <col min="2" max="2" width="12.1328125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="10.796875" style="25" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="25"/>
+    <col min="2" max="2" width="12.140625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="25" customWidth="1"/>
     <col min="4" max="4" width="14" style="25" customWidth="1"/>
-    <col min="5" max="5" width="6.1328125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="17.53125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="10.46484375" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="25"/>
+    <col min="5" max="5" width="6.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>18</v>
@@ -5478,19 +5064,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D5" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G5" s="27">
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -5498,617 +5084,361 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="30"/>
       <c r="C7" s="30" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
         <v>EUR00</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" s="35">
+        <v>76</v>
+      </c>
+      <c r="G7" s="34">
         <f>CPI!$D$21/CPI!D3</f>
         <v>1.3926669328933141</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="32"/>
       <c r="C8" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B4,2))</f>
         <v>EUR01</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G8" s="36">
+        <v>76</v>
+      </c>
+      <c r="G8" s="35">
         <f>CPI!$D$21/CPI!D4</f>
         <v>1.3626878012654737</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="32"/>
       <c r="C9" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B5,2))</f>
         <v>EUR02</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="36">
+        <v>76</v>
+      </c>
+      <c r="G9" s="35">
         <f>CPI!$D$21/CPI!D5</f>
         <v>1.3346599424735295</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="32"/>
       <c r="C10" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B6,2))</f>
         <v>EUR03</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="36">
+        <v>76</v>
+      </c>
+      <c r="G10" s="35">
         <f>CPI!$D$21/CPI!D6</f>
         <v>1.3084901396799309</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B7,2))</f>
         <v>EUR04</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="36">
+        <v>76</v>
+      </c>
+      <c r="G11" s="35">
         <f>CPI!$D$21/CPI!D7</f>
         <v>1.2828334702744419</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="32"/>
       <c r="C12" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B8,2))</f>
         <v>EUR05</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="36">
+        <v>76</v>
+      </c>
+      <c r="G12" s="35">
         <f>CPI!$D$21/CPI!D8</f>
         <v>1.2552186597597279</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
       <c r="C13" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B9,2))</f>
         <v>EUR06</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" s="36">
+        <v>76</v>
+      </c>
+      <c r="G13" s="35">
         <f>CPI!$D$21/CPI!D9</f>
         <v>1.2281982972208687</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
       <c r="C14" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B10,2))</f>
         <v>EUR07</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="36">
+        <v>76</v>
+      </c>
+      <c r="G14" s="35">
         <f>CPI!$D$21/CPI!D10</f>
         <v>1.2005848457682002</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="32"/>
       <c r="C15" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B11,2))</f>
         <v>EUR08</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="36">
+        <v>76</v>
+      </c>
+      <c r="G15" s="35">
         <f>CPI!$D$21/CPI!D11</f>
         <v>1.1577481637108971</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="32"/>
       <c r="C16" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B12,2))</f>
         <v>EUR09</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="36">
+        <v>76</v>
+      </c>
+      <c r="G16" s="35">
         <f>CPI!$D$21/CPI!D12</f>
         <v>1.1462853106048485</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="32"/>
       <c r="C17" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B13,2))</f>
         <v>EUR10</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="36">
+        <v>76</v>
+      </c>
+      <c r="G17" s="35">
         <f>CPI!$D$21/CPI!D13</f>
         <v>1.1227084335013209</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="32"/>
       <c r="C18" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B14,2))</f>
         <v>EUR11</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="36">
+        <v>76</v>
+      </c>
+      <c r="G18" s="35">
         <f>CPI!$D$21/CPI!D14</f>
         <v>1.0889509539295061</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="32"/>
       <c r="C19" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B15,2))</f>
         <v>EUR12</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="36">
+        <v>76</v>
+      </c>
+      <c r="G19" s="35">
         <f>CPI!$D$21/CPI!D15</f>
         <v>1.0613557055843141</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="32"/>
       <c r="C20" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B16,2))</f>
         <v>EUR13</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="36">
+        <v>76</v>
+      </c>
+      <c r="G20" s="35">
         <f>CPI!$D$21/CPI!D16</f>
         <v>1.045670645895876</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="32"/>
       <c r="C21" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B17,2))</f>
         <v>EUR14</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="36">
+        <v>76</v>
+      </c>
+      <c r="G21" s="35">
         <f>CPI!$D$21/CPI!D17</f>
         <v>1.0394340416460002</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="32"/>
       <c r="C22" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B18,2))</f>
         <v>EUR15</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="36">
+        <v>76</v>
+      </c>
+      <c r="G22" s="35">
         <f>CPI!$D$21/CPI!D18</f>
         <v>1.0383956459999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="32"/>
       <c r="C23" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B19,2))</f>
         <v>EUR16</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="32"/>
       <c r="F23" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="36">
+        <v>76</v>
+      </c>
+      <c r="G23" s="35">
         <f>CPI!$D$21/CPI!D19</f>
         <v>1.0363230000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="32"/>
       <c r="C24" s="32" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B20,2))</f>
         <v>EUR17</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" s="36">
+        <v>76</v>
+      </c>
+      <c r="G24" s="35">
         <f>CPI!$D$21/CPI!D20</f>
         <v>1.0190000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="32"/>
       <c r="C25" s="32" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="36">
+        <v>76</v>
+      </c>
+      <c r="G25" s="35">
         <f>CPI!$D$21/CPI!D22</f>
         <v>0.98522167487684731</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B26" s="30" t="str">
-        <f>'Region-Time Slices'!J5</f>
-        <v>SpD</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="37">
-        <f>'Region-Time Slices'!K5</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B27" s="32" t="str">
-        <f>'Region-Time Slices'!J6</f>
-        <v>SpP</v>
-      </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="38">
-        <f>'Region-Time Slices'!K6</f>
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B28" s="32" t="str">
-        <f>'Region-Time Slices'!J7</f>
-        <v>SpE</v>
-      </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="38">
-        <f>'Region-Time Slices'!K7</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B29" s="32" t="str">
-        <f>'Region-Time Slices'!J8</f>
-        <v>SpN</v>
-      </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="38">
-        <f>'Region-Time Slices'!K8</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B30" s="32" t="str">
-        <f>'Region-Time Slices'!J9</f>
-        <v>SuD</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="38">
-        <f>'Region-Time Slices'!K9</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B31" s="32" t="str">
-        <f>'Region-Time Slices'!J10</f>
-        <v>SuP</v>
-      </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="38">
-        <f>'Region-Time Slices'!K10</f>
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B32" s="32" t="str">
-        <f>'Region-Time Slices'!J11</f>
-        <v>SuE</v>
-      </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="38">
-        <f>'Region-Time Slices'!K11</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B33" s="32" t="str">
-        <f>'Region-Time Slices'!J12</f>
-        <v>SuN</v>
-      </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="38">
-        <f>'Region-Time Slices'!K12</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B34" s="32" t="str">
-        <f>'Region-Time Slices'!J13</f>
-        <v>AuD</v>
-      </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="38">
-        <f>'Region-Time Slices'!K13</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B35" s="32" t="str">
-        <f>'Region-Time Slices'!J14</f>
-        <v>AuP</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="38">
-        <f>'Region-Time Slices'!K14</f>
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B36" s="32" t="str">
-        <f>'Region-Time Slices'!J15</f>
-        <v>AuE</v>
-      </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="38">
-        <f>'Region-Time Slices'!K15</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B37" s="32" t="str">
-        <f>'Region-Time Slices'!J16</f>
-        <v>AuN</v>
-      </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="38">
-        <f>'Region-Time Slices'!K16</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B38" s="32" t="str">
-        <f>'Region-Time Slices'!J17</f>
-        <v>WiD</v>
-      </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="38">
-        <f>'Region-Time Slices'!K17</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B39" s="32" t="str">
-        <f>'Region-Time Slices'!J18</f>
-        <v>WiP</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="38">
-        <f>'Region-Time Slices'!K18</f>
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B40" s="32" t="str">
-        <f>'Region-Time Slices'!J19</f>
-        <v>WiE</v>
-      </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="38">
-        <f>'Region-Time Slices'!K19</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B41" s="34" t="str">
-        <f>'Region-Time Slices'!J20</f>
-        <v>WiN</v>
-      </c>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="39">
-        <f>'Region-Time Slices'!K20</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B47" s="27"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B48" s="27"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B49" s="27"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B50" s="28"/>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="27"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="27"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="27"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="28"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="20" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6125,209 +5455,209 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9.1328125" style="25"/>
-    <col min="4" max="4" width="15.53125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="25"/>
+    <col min="1" max="3" width="9.140625" style="25"/>
+    <col min="4" max="4" width="15.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="25" t="str">
         <f>Constants!C7</f>
         <v>EUR00</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="25" t="str">
         <f>Constants!C8</f>
         <v>EUR01</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="25" t="str">
         <f>Constants!C9</f>
         <v>EUR02</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="25" t="str">
         <f>Constants!C10</f>
         <v>EUR03</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="25" t="str">
         <f>Constants!C11</f>
         <v>EUR04</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="25" t="str">
         <f>Constants!C12</f>
         <v>EUR05</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="25" t="str">
         <f>Constants!C13</f>
         <v>EUR06</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="25" t="str">
         <f>Constants!C14</f>
         <v>EUR07</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="str">
         <f>Constants!C15</f>
         <v>EUR08</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="25" t="str">
         <f>Constants!C16</f>
         <v>EUR09</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="25" t="str">
         <f>Constants!C17</f>
         <v>EUR10</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="25" t="str">
         <f>Constants!C18</f>
         <v>EUR11</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="25" t="str">
         <f>Constants!C19</f>
         <v>EUR12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="str">
         <f>Constants!C20</f>
         <v>EUR13</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="25" t="str">
         <f>Constants!C21</f>
         <v>EUR14</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="str">
         <f>Constants!C22</f>
         <v>EUR15</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="str">
         <f>Constants!C23</f>
         <v>EUR16</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="25" t="str">
         <f>Constants!C24</f>
         <v>EUR17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="25" t="str">
         <f>Constants!C25</f>
         <v>EUR19</v>
@@ -6350,24 +5680,24 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="17"/>
-    <col min="2" max="2" width="10.46484375" style="17" customWidth="1"/>
-    <col min="3" max="4" width="13.796875" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="17"/>
+    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="2" max="2" width="10.42578125" style="17" customWidth="1"/>
+    <col min="3" max="4" width="13.85546875" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.2">
       <c r="B2" s="14"/>
       <c r="C2" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="18">
         <v>2000</v>
       </c>
@@ -6376,7 +5706,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="20">
         <v>2001</v>
       </c>
@@ -6388,7 +5718,7 @@
         <v>102.2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="20">
         <v>2002</v>
       </c>
@@ -6400,7 +5730,7 @@
         <v>104.34620000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="20">
         <v>2003</v>
       </c>
@@ -6412,7 +5742,7 @@
         <v>106.43312400000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="20">
         <v>2004</v>
       </c>
@@ -6424,7 +5754,7 @@
         <v>108.56178648000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="20">
         <v>2005</v>
       </c>
@@ -6436,7 +5766,7 @@
         <v>110.95014578256001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="20">
         <v>2006</v>
       </c>
@@ -6448,7 +5778,7 @@
         <v>113.39104898977634</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="20">
         <v>2007</v>
       </c>
@@ -6460,7 +5790,7 @@
         <v>115.99904311654119</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="20">
         <v>2008</v>
       </c>
@@ -6472,7 +5802,7 @@
         <v>120.29100771185321</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="20">
         <v>2009</v>
       </c>
@@ -6484,7 +5814,7 @@
         <v>121.49391778897174</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="20">
         <v>2010</v>
       </c>
@@ -6496,7 +5826,7 @@
         <v>124.04529006254015</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="20">
         <v>2011</v>
       </c>
@@ -6508,7 +5838,7 @@
         <v>127.89069405447889</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="20">
         <v>2012</v>
       </c>
@@ -6520,7 +5850,7 @@
         <v>131.21585209989533</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="20">
         <v>2013</v>
       </c>
@@ -6532,7 +5862,7 @@
         <v>133.18408988139376</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="20">
         <v>2014</v>
       </c>
@@ -6544,11 +5874,11 @@
         <v>133.98319442068211</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="20">
         <v>2015</v>
       </c>
-      <c r="C18" s="70">
+      <c r="C18" s="51">
         <v>1E-3</v>
       </c>
       <c r="D18" s="22">
@@ -6556,57 +5886,57 @@
         <v>134.1171776151028</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="67">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="48">
         <v>2016</v>
       </c>
-      <c r="C19" s="68">
+      <c r="C19" s="49">
         <v>2E-3</v>
       </c>
-      <c r="D19" s="69">
+      <c r="D19" s="50">
         <f t="shared" si="0"/>
         <v>134.385411970333</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="67">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="48">
         <v>2017</v>
       </c>
-      <c r="C20" s="68">
+      <c r="C20" s="49">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D20" s="69">
+      <c r="D20" s="50">
         <f t="shared" si="0"/>
         <v>136.66996397382866</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="67">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="48">
         <v>2018</v>
       </c>
-      <c r="C21" s="68">
+      <c r="C21" s="49">
         <v>1.9E-2</v>
       </c>
-      <c r="D21" s="69">
+      <c r="D21" s="50">
         <f t="shared" si="0"/>
         <v>139.26669328933141</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="67">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="48">
         <v>2019</v>
       </c>
-      <c r="C22" s="68">
+      <c r="C22" s="49">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D22" s="69">
+      <c r="D22" s="50">
         <f t="shared" si="0"/>
         <v>141.35569368867138</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -6616,6 +5946,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327522a6d5518d67d5f1063e9cc64cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd5532d255be23b9fb13183c07e1fd0" ns2:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -6761,22 +6106,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA920D49-9FB9-4142-A1B8-91AD121D6293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD240B5B-3D13-4D9E-8A01-EF772CCE06DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C39DA6-9ADC-4432-AC8D-D99B3FEDE92E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6792,21 +6139,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD240B5B-3D13-4D9E-8A01-EF772CCE06DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA920D49-9FB9-4142-A1B8-91AD121D6293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Use 16 time slices
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,26 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9938C528-DEA8-4E8C-BF72-13CE42EE050F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Regions" sheetId="27" r:id="rId1"/>
-    <sheet name="Region-Time Slices" sheetId="20" r:id="rId2"/>
-    <sheet name="TimePeriods" sheetId="24" r:id="rId3"/>
-    <sheet name="Import Settings" sheetId="17" r:id="rId4"/>
-    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId5"/>
-    <sheet name="Constants" sheetId="25" r:id="rId6"/>
-    <sheet name="Defaults" sheetId="26" r:id="rId7"/>
-    <sheet name="CPI" sheetId="23" r:id="rId8"/>
+    <sheet name="Regions" sheetId="27" state="visible" r:id="rId1"/>
+    <sheet name="Region-Time Slices" sheetId="20" state="visible" r:id="rId2"/>
+    <sheet name="TimePeriods" sheetId="24" state="visible" r:id="rId3"/>
+    <sheet name="Import Settings" sheetId="17" state="visible" r:id="rId4"/>
+    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" state="visible" r:id="rId5"/>
+    <sheet name="Constants" sheetId="25" state="visible" r:id="rId6"/>
+    <sheet name="Defaults" sheetId="26" state="visible" r:id="rId7"/>
+    <sheet name="CPI" sheetId="23" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -34,22 +27,11 @@
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -473,15 +455,54 @@
   <si>
     <t>Hour</t>
   </si>
+  <si>
+    <t xml:space="preserve">Wi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Su</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hour</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -492,12 +513,28 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="10"/>
@@ -507,41 +544,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
       <sz val="10"/>
@@ -550,12 +571,12 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="14"/>
@@ -565,12 +586,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="10"/>
@@ -594,17 +615,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="10">
@@ -672,24 +688,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -698,11 +707,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -717,7 +724,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -726,25 +732,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -754,16 +754,11 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -778,7 +773,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -795,10 +789,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -814,9 +808,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -832,10 +826,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -844,13 +838,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,7 +852,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -870,12 +863,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -991,7 +980,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -1832,7 +1821,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -2229,7 +2218,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2406,7 +2395,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2628,7 +2617,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -3080,7 +3069,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -3268,31 +3257,31 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="season_info" displayName="season_info" ref="K4:L16" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="season_info" displayName="season_info" ref="K4:L16" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Month"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Season"/>
+    <tableColumn id="1" name="Month"/>
+    <tableColumn id="2" name="Season"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="weekly_info" displayName="weekly_info" ref="N4:O11" totalsRowShown="0">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="weekly_info" displayName="weekly_info" ref="N4:O11" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Day"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Type"/>
+    <tableColumn id="1" name="Day"/>
+    <tableColumn id="2" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="daynite_info" displayName="daynite_info" ref="Q4:R28" totalsRowShown="0">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="daynite_info" displayName="daynite_info" ref="Q4:R28" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
+    <tableColumn id="1" name="Hour"/>
+    <tableColumn id="2" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3618,45 +3607,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AD37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1"/>
-    <col min="23" max="23" width="5" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" customWidth="1"/>
-    <col min="26" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="5" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="6" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="18" max="18" width="6" hidden="0" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" hidden="0" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="23" max="23" width="5" hidden="0" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="6" hidden="0" customWidth="1"/>
+    <col min="27" max="27" width="6" hidden="0" customWidth="1"/>
+    <col min="28" max="28" width="6" hidden="0" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="15" customHeight="1">
       <c r="C3" s="2" t="str">
         <f t="array" ref="C3">IF(INDEX(C5:C7,$A$4)&lt;&gt;0,INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -3770,13 +3762,13 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3891,7 +3883,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3927,7 +3919,7 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -4041,7 +4033,7 @@
       </c>
       <c r="AD7" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -4049,7 +4041,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="4" t="s">
         <v>76</v>
       </c>
@@ -4057,7 +4049,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="5" t="s">
         <v>78</v>
       </c>
@@ -4065,7 +4057,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="5" t="s">
         <v>80</v>
       </c>
@@ -4073,7 +4065,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="5" t="s">
         <v>82</v>
       </c>
@@ -4081,7 +4073,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="5" t="s">
         <v>84</v>
       </c>
@@ -4089,7 +4081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -4097,7 +4089,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
@@ -4105,7 +4097,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
@@ -4113,7 +4105,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="5" t="s">
         <v>92</v>
       </c>
@@ -4121,7 +4113,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="5" t="s">
         <v>94</v>
       </c>
@@ -4129,7 +4121,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="5" t="s">
         <v>96</v>
       </c>
@@ -4137,7 +4129,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="5" t="s">
         <v>98</v>
       </c>
@@ -4145,7 +4137,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
@@ -4153,7 +4145,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="5" t="s">
         <v>102</v>
       </c>
@@ -4161,7 +4153,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="5" t="s">
         <v>104</v>
       </c>
@@ -4169,7 +4161,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="5" t="s">
         <v>106</v>
       </c>
@@ -4177,7 +4169,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="5" t="s">
         <v>108</v>
       </c>
@@ -4185,7 +4177,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="5" t="s">
         <v>110</v>
       </c>
@@ -4193,7 +4185,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="5" t="s">
         <v>112</v>
       </c>
@@ -4201,7 +4193,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="5" t="s">
         <v>114</v>
       </c>
@@ -4209,7 +4201,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="5" t="s">
         <v>116</v>
       </c>
@@ -4217,7 +4209,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="5" t="s">
         <v>118</v>
       </c>
@@ -4225,7 +4217,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="5" t="s">
         <v>120</v>
       </c>
@@ -4233,7 +4225,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="5" t="s">
         <v>122</v>
       </c>
@@ -4241,7 +4233,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="5" t="s">
         <v>124</v>
       </c>
@@ -4249,7 +4241,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="5" t="s">
         <v>126</v>
       </c>
@@ -4257,7 +4249,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>128</v>
       </c>
@@ -4266,680 +4258,664 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2" r:id="rId3" name="Drop Down 1">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <legacyDrawing r:id="rIdvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:AB39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="11" t="s">
+    <row r="3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="9" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="L4" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="N4" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="O4" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="Q4" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="R4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="8" t="str">
+      <c r="C5" s="10" t="str">
         <f>Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="K5">
+      <c r="E5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>129</v>
-      </c>
-      <c r="N5">
+        <v>135</v>
+      </c>
+      <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q5">
+        <v>139</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="str">
         <f>Regions!D3</f>
         <v>National</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="K6">
+      <c r="E6" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" t="n">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>129</v>
-      </c>
-      <c r="N6">
+        <v>135</v>
+      </c>
+      <c r="N6" t="n">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q6">
+        <v>139</v>
+      </c>
+      <c r="Q6" t="n">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="str">
         <f>Regions!E3</f>
         <v>IE-CW</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="K7">
+      <c r="E7" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7" t="n">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>129</v>
-      </c>
-      <c r="N7">
+        <v>136</v>
+      </c>
+      <c r="N7" t="n">
         <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q7">
+        <v>139</v>
+      </c>
+      <c r="Q7" t="n">
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="str">
         <f>Regions!F3</f>
         <v>IE-D</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="K8">
+      <c r="E8" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="K8" t="n">
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>129</v>
-      </c>
-      <c r="N8">
+        <v>136</v>
+      </c>
+      <c r="N8" t="n">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q8">
+        <v>139</v>
+      </c>
+      <c r="Q8" t="n">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="str">
         <f>Regions!G3</f>
         <v>IE-KE</v>
       </c>
-      <c r="K9">
+      <c r="K9" t="n">
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>129</v>
-      </c>
-      <c r="N9">
+        <v>136</v>
+      </c>
+      <c r="N9" t="n">
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q9">
+        <v>139</v>
+      </c>
+      <c r="Q9" t="n">
         <v>4</v>
       </c>
       <c r="R9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="str">
         <f>Regions!H3</f>
         <v>IE-KK</v>
       </c>
-      <c r="K10">
+      <c r="K10" t="n">
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>129</v>
-      </c>
-      <c r="N10">
+        <v>137</v>
+      </c>
+      <c r="N10" t="n">
         <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q10">
+        <v>139</v>
+      </c>
+      <c r="Q10" t="n">
         <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10" t="str">
         <f>Regions!I3</f>
         <v>IE-LS</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="K11">
+      <c r="E11" s="9"/>
+      <c r="K11" t="n">
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>129</v>
-      </c>
-      <c r="N11">
+        <v>137</v>
+      </c>
+      <c r="N11" t="n">
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q11">
+        <v>139</v>
+      </c>
+      <c r="Q11" t="n">
         <v>6</v>
       </c>
       <c r="R11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="str">
         <f>Regions!J3</f>
         <v>IE-LD</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="K12">
+      <c r="E12" s="9"/>
+      <c r="K12" t="n">
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q12">
+        <v>137</v>
+      </c>
+      <c r="Q12" t="n">
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="str">
         <f>Regions!K3</f>
         <v>IE-LH</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="K13">
+      <c r="E13" s="9"/>
+      <c r="K13" t="n">
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q13">
+        <v>138</v>
+      </c>
+      <c r="Q13" t="n">
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="str">
         <f>Regions!L3</f>
         <v>IE-MH</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="K14">
+      <c r="E14" s="9"/>
+      <c r="K14" t="n">
         <v>9</v>
       </c>
       <c r="L14" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q14">
+        <v>138</v>
+      </c>
+      <c r="Q14" t="n">
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10" t="str">
         <f>Regions!M3</f>
         <v>IE-OY</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="K15">
+      <c r="E15" s="9"/>
+      <c r="K15" t="n">
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q15">
+        <v>138</v>
+      </c>
+      <c r="Q15" t="n">
         <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10" t="str">
         <f>Regions!N3</f>
         <v>IE-WH</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="K16">
+      <c r="E16" s="9"/>
+      <c r="K16" t="n">
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q16">
+        <v>135</v>
+      </c>
+      <c r="Q16" t="n">
         <v>11</v>
       </c>
       <c r="R16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="str">
         <f>Regions!O3</f>
         <v>IE-WX</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="Q17">
+      <c r="E17" s="9"/>
+      <c r="Q17" t="n">
         <v>12</v>
       </c>
       <c r="R17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="str">
         <f>Regions!P3</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" t="n">
         <v>13</v>
       </c>
       <c r="R18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10" t="str">
         <f>Regions!Q3</f>
         <v>IE-CE</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" t="n">
         <v>14</v>
       </c>
       <c r="R19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="C20" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9"/>
+      <c r="C20" s="10" t="str">
         <f>Regions!R3</f>
         <v>IE-CO</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" t="n">
         <v>15</v>
       </c>
       <c r="R20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="C21" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9"/>
+      <c r="C21" s="10" t="str">
         <f>Regions!S3</f>
         <v>IE-KY</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" t="n">
         <v>16</v>
       </c>
       <c r="R21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="C22" s="8" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9"/>
+      <c r="C22" s="10" t="str">
         <f>Regions!T3</f>
         <v>IE-LK</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" t="n">
         <v>17</v>
       </c>
       <c r="R22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="C23" s="8" t="str">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9"/>
+      <c r="C23" s="10" t="str">
         <f>Regions!U3</f>
         <v>IE-TA</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" t="n">
         <v>18</v>
       </c>
       <c r="R23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="C24" s="8" t="str">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9"/>
+      <c r="C24" s="10" t="str">
         <f>Regions!V3</f>
         <v>IE-WD</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" t="n">
         <v>19</v>
       </c>
       <c r="R24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="C25" s="8" t="str">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9"/>
+      <c r="C25" s="10" t="str">
         <f>Regions!W3</f>
         <v>IE-G</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" t="n">
         <v>20</v>
       </c>
       <c r="R25" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="C26" s="8" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9"/>
+      <c r="C26" s="10" t="str">
         <f>Regions!X3</f>
         <v>IE-LM</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" t="n">
         <v>21</v>
       </c>
       <c r="R26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="C27" s="8" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9"/>
+      <c r="C27" s="10" t="str">
         <f>Regions!Y3</f>
         <v>IE-MO</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" t="n">
         <v>22</v>
       </c>
       <c r="R27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="C28" s="8" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="9"/>
+      <c r="C28" s="10" t="str">
         <f>Regions!Z3</f>
         <v>IE-RN</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" t="n">
         <v>23</v>
       </c>
       <c r="R28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="C29" s="8" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9"/>
+      <c r="C29" s="10" t="str">
         <f>Regions!AA3</f>
         <v>IE-SO</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="C30" s="8" t="str">
+    <row r="30">
+      <c r="A30" s="9"/>
+      <c r="C30" s="10" t="str">
         <f>Regions!AB3</f>
         <v>IE-CN</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="C31" s="8" t="str">
+    <row r="31">
+      <c r="A31" s="9"/>
+      <c r="C31" s="10" t="str">
         <f>Regions!AC3</f>
         <v>IE-DL</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="C32" s="8" t="str">
+    <row r="32">
+      <c r="A32" s="9"/>
+      <c r="C32" s="10" t="str">
         <f>Regions!AD3</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="8"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+    <row r="33">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="9"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="10"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="9"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="9"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="9"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4">
+    <row r="4">
+      <c r="B4" t="n">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="14" t="s">
         <v>67</v>
       </c>
@@ -4947,117 +4923,117 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="13">
+    <row r="13">
+      <c r="B13" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="13">
+    <row r="14">
+      <c r="B14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="13">
+    <row r="15">
+      <c r="B15" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="13">
+    <row r="16">
+      <c r="B16" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="13">
+    <row r="17">
+      <c r="B17" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="13">
+    <row r="18">
+      <c r="B18" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
+    <row r="19">
+      <c r="B19" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
+    <row r="20">
+      <c r="B20" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
+    <row r="21">
+      <c r="B21" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="13">
+    <row r="22">
+      <c r="B22" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="13">
+    <row r="23">
+      <c r="B23" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="13">
+    <row r="24">
+      <c r="B24" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="B25" s="13"/>
-      <c r="C25" s="13">
+      <c r="C25" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="B26" s="13"/>
-      <c r="C26" s="13">
+      <c r="C26" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="B27" s="13"/>
-      <c r="C27" s="13">
+      <c r="C27" s="13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5069,24 +5045,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B3:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
@@ -5094,43 +5070,43 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="B5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="19" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="13" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="B9" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5142,49 +5118,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="24"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2">
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3">
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -5202,7 +5178,7 @@
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5220,7 +5196,7 @@
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -5238,7 +5214,7 @@
       <c r="O10" s="26"/>
       <c r="P10" s="26"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -5256,7 +5232,7 @@
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -5274,7 +5250,7 @@
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="18.75" customHeight="1">
       <c r="A13" s="20" t="s">
         <v>56</v>
       </c>
@@ -5293,7 +5269,7 @@
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="25" t="s">
         <v>0</v>
       </c>
@@ -5313,7 +5289,7 @@
       <c r="O14" s="26"/>
       <c r="P14" s="26"/>
     </row>
-    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
@@ -5363,7 +5339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26" t="s">
@@ -5371,7 +5347,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="26">
+      <c r="F16" s="26" t="n">
         <v>2222</v>
       </c>
       <c r="G16" s="26"/>
@@ -5389,7 +5365,7 @@
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26" t="s">
@@ -5397,7 +5373,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="26">
+      <c r="F17" s="26" t="n">
         <v>8888</v>
       </c>
       <c r="G17" s="26"/>
@@ -5415,7 +5391,7 @@
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -5433,7 +5409,7 @@
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -5451,7 +5427,7 @@
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -5469,7 +5445,7 @@
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -5487,7 +5463,7 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -5505,7 +5481,7 @@
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -5523,7 +5499,7 @@
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -5549,62 +5525,62 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="14" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="B1" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
+    <row r="3">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D5" s="7" t="s">
+    <row r="5">
+      <c r="D5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="9" t="n">
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28" t="s">
@@ -5612,11 +5588,11 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
-      <c r="G6" s="28">
+      <c r="G6" s="28" t="n">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
@@ -5629,344 +5605,344 @@
       <c r="F7" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="29" t="n">
         <f>CPI!$D$21/CPI!D3</f>
         <v>1.3926669328933141</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="str">
+    <row r="8">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B4,2))</f>
         <v>EUR01</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="27" t="n">
         <f>CPI!$D$21/CPI!D4</f>
         <v>1.3626878012654737</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="str">
+    <row r="9">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B5,2))</f>
         <v>EUR02</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="27" t="n">
         <f>CPI!$D$21/CPI!D5</f>
         <v>1.3346599424735295</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="str">
+    <row r="10">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B6,2))</f>
         <v>EUR03</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="27" t="n">
         <f>CPI!$D$21/CPI!D6</f>
         <v>1.3084901396799309</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="str">
+    <row r="11">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B7,2))</f>
         <v>EUR04</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="27" t="n">
         <f>CPI!$D$21/CPI!D7</f>
         <v>1.2828334702744419</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="str">
+    <row r="12">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B8,2))</f>
         <v>EUR05</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="27" t="n">
         <f>CPI!$D$21/CPI!D8</f>
         <v>1.2552186597597279</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="str">
+    <row r="13">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B9,2))</f>
         <v>EUR06</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="27" t="n">
         <f>CPI!$D$21/CPI!D9</f>
         <v>1.2281982972208687</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="str">
+    <row r="14">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B10,2))</f>
         <v>EUR07</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="27" t="n">
         <f>CPI!$D$21/CPI!D10</f>
         <v>1.2005848457682002</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="str">
+    <row r="15">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B11,2))</f>
         <v>EUR08</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="27" t="n">
         <f>CPI!$D$21/CPI!D11</f>
         <v>1.1577481637108971</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="str">
+    <row r="16">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B12,2))</f>
         <v>EUR09</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="27" t="n">
         <f>CPI!$D$21/CPI!D12</f>
         <v>1.1462853106048485</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7" t="str">
+    <row r="17">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B13,2))</f>
         <v>EUR10</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="27" t="n">
         <f>CPI!$D$21/CPI!D13</f>
         <v>1.1227084335013209</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7" t="str">
+    <row r="18">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B14,2))</f>
         <v>EUR11</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="27" t="n">
         <f>CPI!$D$21/CPI!D14</f>
         <v>1.0889509539295061</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="str">
+    <row r="19">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B15,2))</f>
         <v>EUR12</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="27" t="n">
         <f>CPI!$D$21/CPI!D15</f>
         <v>1.0613557055843141</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="str">
+    <row r="20">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B16,2))</f>
         <v>EUR13</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="27" t="n">
         <f>CPI!$D$21/CPI!D16</f>
         <v>1.045670645895876</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="str">
+    <row r="21">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B17,2))</f>
         <v>EUR14</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="27" t="n">
         <f>CPI!$D$21/CPI!D17</f>
         <v>1.0394340416460002</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7" t="str">
+    <row r="22">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B18,2))</f>
         <v>EUR15</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="27" t="n">
         <f>CPI!$D$21/CPI!D18</f>
         <v>1.0383956459999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7" t="str">
+    <row r="23">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B19,2))</f>
         <v>EUR16</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="27" t="n">
         <f>CPI!$D$21/CPI!D19</f>
         <v>1.0363230000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7" t="str">
+    <row r="24">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B20,2))</f>
         <v>EUR17</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="27" t="n">
         <f>CPI!$D$21/CPI!D20</f>
         <v>1.0190000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7" t="s">
+    <row r="25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="27" t="n">
         <f>CPI!$D$21/CPI!D22</f>
         <v>0.98522167487684731</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="9"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34">
       <c r="B34" s="27"/>
     </row>
   </sheetData>
@@ -5977,215 +5953,215 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+    <row r="2">
+      <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="B3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
+    <row r="4">
+      <c r="B4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="str">
+    <row r="5">
+      <c r="B5" s="9" t="str">
         <f>Constants!C7</f>
         <v>EUR00</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="str">
+    <row r="6">
+      <c r="B6" s="9" t="str">
         <f>Constants!C8</f>
         <v>EUR01</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="str">
+    <row r="7">
+      <c r="B7" s="9" t="str">
         <f>Constants!C9</f>
         <v>EUR02</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="str">
+    <row r="8">
+      <c r="B8" s="9" t="str">
         <f>Constants!C10</f>
         <v>EUR03</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="str">
+    <row r="9">
+      <c r="B9" s="9" t="str">
         <f>Constants!C11</f>
         <v>EUR04</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="str">
+    <row r="10">
+      <c r="B10" s="9" t="str">
         <f>Constants!C12</f>
         <v>EUR05</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="str">
+    <row r="11">
+      <c r="B11" s="9" t="str">
         <f>Constants!C13</f>
         <v>EUR06</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="str">
+    <row r="12">
+      <c r="B12" s="9" t="str">
         <f>Constants!C14</f>
         <v>EUR07</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="str">
+    <row r="13">
+      <c r="B13" s="9" t="str">
         <f>Constants!C15</f>
         <v>EUR08</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="str">
+    <row r="14">
+      <c r="B14" s="9" t="str">
         <f>Constants!C16</f>
         <v>EUR09</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="str">
+    <row r="15">
+      <c r="B15" s="9" t="str">
         <f>Constants!C17</f>
         <v>EUR10</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="str">
+    <row r="16">
+      <c r="B16" s="9" t="str">
         <f>Constants!C18</f>
         <v>EUR11</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="str">
+    <row r="17">
+      <c r="B17" s="9" t="str">
         <f>Constants!C19</f>
         <v>EUR12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="str">
+    <row r="18">
+      <c r="B18" s="9" t="str">
         <f>Constants!C20</f>
         <v>EUR13</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="str">
+    <row r="19">
+      <c r="B19" s="9" t="str">
         <f>Constants!C21</f>
         <v>EUR14</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="str">
+    <row r="20">
+      <c r="B20" s="9" t="str">
         <f>Constants!C22</f>
         <v>EUR15</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="str">
+    <row r="21">
+      <c r="B21" s="9" t="str">
         <f>Constants!C23</f>
         <v>EUR16</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="7" t="str">
+    <row r="22">
+      <c r="B22" s="9" t="str">
         <f>Constants!C24</f>
         <v>EUR17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="str">
+    <row r="23">
+      <c r="B23" s="9" t="str">
         <f>Constants!C25</f>
         <v>EUR19</v>
       </c>
@@ -6198,20 +6174,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B2:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="30" customHeight="1">
       <c r="B2" s="30"/>
       <c r="C2" s="31" t="s">
         <v>38</v>
@@ -6220,244 +6197,244 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="33">
+    <row r="3" ht="15" customHeight="1">
+      <c r="B3" s="33" t="n">
         <v>2000</v>
       </c>
       <c r="C3" s="34"/>
-      <c r="D3" s="34">
+      <c r="D3" s="34" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="33">
+    <row r="4" ht="15" customHeight="1">
+      <c r="B4" s="33" t="n">
         <v>2001</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="34" t="n">
         <f t="shared" ref="D4:D22" si="0">D3+D3*C4</f>
         <v>102.2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="33">
+    <row r="5" ht="15" customHeight="1">
+      <c r="B5" s="33" t="n">
         <v>2002</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="35" t="n">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="36" t="n">
         <f t="shared" si="0"/>
         <v>104.34620000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="33">
+    <row r="6" ht="15" customHeight="1">
+      <c r="B6" s="33" t="n">
         <v>2003</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="35" t="n">
         <v>0.02</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="36" t="n">
         <f t="shared" si="0"/>
         <v>106.43312400000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="33">
+    <row r="7" ht="15" customHeight="1">
+      <c r="B7" s="33" t="n">
         <v>2004</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="35" t="n">
         <v>0.02</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="36" t="n">
         <f t="shared" si="0"/>
         <v>108.56178648000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="33">
+    <row r="8" ht="15" customHeight="1">
+      <c r="B8" s="33" t="n">
         <v>2005</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="36" t="n">
         <f t="shared" si="0"/>
         <v>110.95014578256001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="33">
+    <row r="9" ht="15" customHeight="1">
+      <c r="B9" s="33" t="n">
         <v>2006</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="36" t="n">
         <f t="shared" si="0"/>
         <v>113.39104898977634</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="33">
+    <row r="10" ht="15" customHeight="1">
+      <c r="B10" s="33" t="n">
         <v>2007</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="35" t="n">
         <v>2.3E-2</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="36" t="n">
         <f t="shared" si="0"/>
         <v>115.99904311654119</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="33">
+    <row r="11" ht="15" customHeight="1">
+      <c r="B11" s="33" t="n">
         <v>2008</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="35" t="n">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="36" t="n">
         <f t="shared" si="0"/>
         <v>120.29100771185321</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="33">
+    <row r="12" ht="15" customHeight="1">
+      <c r="B12" s="33" t="n">
         <v>2009</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="35" t="n">
         <v>0.01</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="36" t="n">
         <f t="shared" si="0"/>
         <v>121.49391778897174</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="33">
+    <row r="13" ht="15" customHeight="1">
+      <c r="B13" s="33" t="n">
         <v>2010</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="35" t="n">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="36" t="n">
         <f t="shared" si="0"/>
         <v>124.04529006254015</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="33">
+    <row r="14" ht="15" customHeight="1">
+      <c r="B14" s="33" t="n">
         <v>2011</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="35" t="n">
         <v>3.1E-2</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="36" t="n">
         <f t="shared" si="0"/>
         <v>127.89069405447889</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="33">
+    <row r="15" ht="15" customHeight="1">
+      <c r="B15" s="33" t="n">
         <v>2012</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="35" t="n">
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="36" t="n">
         <f t="shared" si="0"/>
         <v>131.21585209989533</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="33">
+    <row r="16" ht="15" customHeight="1">
+      <c r="B16" s="33" t="n">
         <v>2013</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="35" t="n">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="36" t="n">
         <f t="shared" si="0"/>
         <v>133.18408988139376</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="33">
+    <row r="17" ht="15" customHeight="1">
+      <c r="B17" s="33" t="n">
         <v>2014</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="35" t="n">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="36" t="n">
         <f t="shared" si="0"/>
         <v>133.98319442068211</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="33">
+    <row r="18" ht="15" customHeight="1">
+      <c r="B18" s="33" t="n">
         <v>2015</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="41" t="n">
         <v>1E-3</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="36" t="n">
         <f>D17+D17*C18</f>
         <v>134.1171776151028</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="38">
+    <row r="19" ht="15" customHeight="1">
+      <c r="B19" s="38" t="n">
         <v>2016</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="39" t="n">
         <v>2E-3</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="40" t="n">
         <f t="shared" si="0"/>
         <v>134.385411970333</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="38">
+    <row r="20" ht="15" customHeight="1">
+      <c r="B20" s="38" t="n">
         <v>2017</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="39" t="n">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="40" t="n">
         <f t="shared" si="0"/>
         <v>136.66996397382866</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
+    <row r="21" ht="15" customHeight="1">
+      <c r="B21" s="38" t="n">
         <v>2018</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="39" t="n">
         <v>1.9E-2</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="40" t="n">
         <f t="shared" si="0"/>
         <v>139.26669328933141</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="38">
+    <row r="22" ht="15" customHeight="1">
+      <c r="B22" s="38" t="n">
         <v>2019</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="39" t="n">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="40" t="n">
         <f t="shared" si="0"/>
         <v>141.35569368867138</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" ht="15" customHeight="1">
       <c r="B24" s="37" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Change to 8760 ts
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,26 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9938C528-DEA8-4E8C-BF72-13CE42EE050F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Regions" sheetId="27" r:id="rId1"/>
-    <sheet name="Region-Time Slices" sheetId="20" r:id="rId2"/>
-    <sheet name="TimePeriods" sheetId="24" r:id="rId3"/>
-    <sheet name="Import Settings" sheetId="17" r:id="rId4"/>
-    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId5"/>
-    <sheet name="Constants" sheetId="25" r:id="rId6"/>
-    <sheet name="Defaults" sheetId="26" r:id="rId7"/>
-    <sheet name="CPI" sheetId="23" r:id="rId8"/>
+    <sheet name="Regions" sheetId="27" state="visible" r:id="rId1"/>
+    <sheet name="Region-Time Slices" sheetId="20" state="visible" r:id="rId2"/>
+    <sheet name="TimePeriods" sheetId="24" state="visible" r:id="rId3"/>
+    <sheet name="Import Settings" sheetId="17" state="visible" r:id="rId4"/>
+    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" state="visible" r:id="rId5"/>
+    <sheet name="Constants" sheetId="25" state="visible" r:id="rId6"/>
+    <sheet name="Defaults" sheetId="26" state="visible" r:id="rId7"/>
+    <sheet name="CPI" sheetId="23" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -34,22 +27,11 @@
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -473,15 +455,159 @@
   <si>
     <t>Hour</t>
   </si>
+  <si>
+    <t xml:space="preserve">Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hour</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -492,12 +618,28 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="10"/>
@@ -507,41 +649,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
       <sz val="10"/>
@@ -550,12 +676,12 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="14"/>
@@ -565,12 +691,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="10"/>
@@ -594,17 +720,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="10">
@@ -672,24 +793,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -698,11 +812,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -717,7 +829,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -726,25 +837,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -754,16 +859,11 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -778,7 +878,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -795,10 +894,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -814,9 +913,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -832,10 +931,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -844,13 +943,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,7 +957,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -870,12 +968,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -991,7 +1085,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -1832,7 +1926,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -2229,7 +2323,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2406,7 +2500,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2628,7 +2722,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -3080,7 +3174,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -3268,31 +3362,31 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="season_info" displayName="season_info" ref="K4:L16" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="season_info" displayName="season_info" ref="K4:L16" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Month"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Season"/>
+    <tableColumn id="1" name="Month"/>
+    <tableColumn id="2" name="Season"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="weekly_info" displayName="weekly_info" ref="N4:O11" totalsRowShown="0">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="weekly_info" displayName="weekly_info" ref="N4:O11" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Day"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Type"/>
+    <tableColumn id="1" name="Day"/>
+    <tableColumn id="2" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="daynite_info" displayName="daynite_info" ref="Q4:R28" totalsRowShown="0">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="daynite_info" displayName="daynite_info" ref="Q4:R28" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
+    <tableColumn id="1" name="Hour"/>
+    <tableColumn id="2" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3618,45 +3712,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AD37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1"/>
-    <col min="23" max="23" width="5" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" customWidth="1"/>
-    <col min="26" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="5" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="6" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="18" max="18" width="6" hidden="0" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" hidden="0" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="23" max="23" width="5" hidden="0" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="6" hidden="0" customWidth="1"/>
+    <col min="27" max="27" width="6" hidden="0" customWidth="1"/>
+    <col min="28" max="28" width="6" hidden="0" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="15" customHeight="1">
       <c r="C3" s="2" t="str">
         <f t="array" ref="C3">IF(INDEX(C5:C7,$A$4)&lt;&gt;0,INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -3770,13 +3867,13 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3891,7 +3988,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3927,7 +4024,7 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -4041,7 +4138,7 @@
       </c>
       <c r="AD7" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -4049,7 +4146,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="4" t="s">
         <v>76</v>
       </c>
@@ -4057,7 +4154,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="5" t="s">
         <v>78</v>
       </c>
@@ -4065,7 +4162,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="5" t="s">
         <v>80</v>
       </c>
@@ -4073,7 +4170,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="5" t="s">
         <v>82</v>
       </c>
@@ -4081,7 +4178,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="5" t="s">
         <v>84</v>
       </c>
@@ -4089,7 +4186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -4097,7 +4194,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
@@ -4105,7 +4202,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
@@ -4113,7 +4210,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="5" t="s">
         <v>92</v>
       </c>
@@ -4121,7 +4218,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="5" t="s">
         <v>94</v>
       </c>
@@ -4129,7 +4226,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="5" t="s">
         <v>96</v>
       </c>
@@ -4137,7 +4234,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="5" t="s">
         <v>98</v>
       </c>
@@ -4145,7 +4242,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
@@ -4153,7 +4250,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="5" t="s">
         <v>102</v>
       </c>
@@ -4161,7 +4258,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="5" t="s">
         <v>104</v>
       </c>
@@ -4169,7 +4266,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="5" t="s">
         <v>106</v>
       </c>
@@ -4177,7 +4274,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="5" t="s">
         <v>108</v>
       </c>
@@ -4185,7 +4282,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="5" t="s">
         <v>110</v>
       </c>
@@ -4193,7 +4290,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="5" t="s">
         <v>112</v>
       </c>
@@ -4201,7 +4298,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="5" t="s">
         <v>114</v>
       </c>
@@ -4209,7 +4306,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="5" t="s">
         <v>116</v>
       </c>
@@ -4217,7 +4314,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="5" t="s">
         <v>118</v>
       </c>
@@ -4225,7 +4322,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="5" t="s">
         <v>120</v>
       </c>
@@ -4233,7 +4330,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="5" t="s">
         <v>122</v>
       </c>
@@ -4241,7 +4338,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="5" t="s">
         <v>124</v>
       </c>
@@ -4249,7 +4346,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="5" t="s">
         <v>126</v>
       </c>
@@ -4257,7 +4354,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>128</v>
       </c>
@@ -4266,680 +4363,785 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2" r:id="rId3" name="Drop Down 1">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <legacyDrawing r:id="rIdvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:AB39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="11" t="s">
+    <row r="3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="9" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="L4" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="N4" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="O4" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="Q4" t="s">
-        <v>134</v>
+        <v>182</v>
       </c>
       <c r="R4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="8" t="str">
+      <c r="C5" s="10" t="str">
         <f>Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="K5">
+      <c r="E5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>129</v>
-      </c>
-      <c r="N5">
+        <v>135</v>
+      </c>
+      <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q5">
+        <v>153</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="str">
         <f>Regions!D3</f>
         <v>National</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="K6">
+      <c r="E6" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" t="n">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>129</v>
-      </c>
-      <c r="N6">
+        <v>136</v>
+      </c>
+      <c r="N6" t="n">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q6">
+        <v>147</v>
+      </c>
+      <c r="Q6" t="n">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="str">
         <f>Regions!E3</f>
         <v>IE-CW</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="K7">
+      <c r="E7" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="K7" t="n">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>129</v>
-      </c>
-      <c r="N7">
+        <v>137</v>
+      </c>
+      <c r="N7" t="n">
         <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q7">
+        <v>148</v>
+      </c>
+      <c r="Q7" t="n">
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8" t="str">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="str">
         <f>Regions!F3</f>
         <v>IE-D</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="K8">
+      <c r="E8" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="K8" t="n">
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>129</v>
-      </c>
-      <c r="N8">
+        <v>138</v>
+      </c>
+      <c r="N8" t="n">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q8">
+        <v>149</v>
+      </c>
+      <c r="Q8" t="n">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="str">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="str">
         <f>Regions!G3</f>
         <v>IE-KE</v>
       </c>
-      <c r="K9">
+      <c r="E9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K9" t="n">
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>129</v>
-      </c>
-      <c r="N9">
+        <v>139</v>
+      </c>
+      <c r="N9" t="n">
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q9">
+        <v>150</v>
+      </c>
+      <c r="Q9" t="n">
         <v>4</v>
       </c>
       <c r="R9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8" t="str">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="str">
         <f>Regions!H3</f>
         <v>IE-KK</v>
       </c>
-      <c r="K10">
+      <c r="E10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K10" t="n">
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>129</v>
-      </c>
-      <c r="N10">
+        <v>140</v>
+      </c>
+      <c r="N10" t="n">
         <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q10">
+        <v>151</v>
+      </c>
+      <c r="Q10" t="n">
         <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="str">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10" t="str">
         <f>Regions!I3</f>
         <v>IE-LS</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="K11">
+      <c r="E11" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K11" t="n">
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>129</v>
-      </c>
-      <c r="N11">
+        <v>141</v>
+      </c>
+      <c r="N11" t="n">
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q11">
+        <v>152</v>
+      </c>
+      <c r="Q11" t="n">
         <v>6</v>
       </c>
       <c r="R11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8" t="str">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="str">
         <f>Regions!J3</f>
         <v>IE-LD</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="K12">
+      <c r="E12" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12" t="s">
+        <v>161</v>
+      </c>
+      <c r="K12" t="n">
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q12">
+        <v>142</v>
+      </c>
+      <c r="Q12" t="n">
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8" t="str">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="str">
         <f>Regions!K3</f>
         <v>IE-LH</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="K13">
+      <c r="E13" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13"/>
+      <c r="G13" t="s">
+        <v>162</v>
+      </c>
+      <c r="K13" t="n">
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q13">
+        <v>143</v>
+      </c>
+      <c r="Q13" t="n">
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8" t="str">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="str">
         <f>Regions!L3</f>
         <v>IE-MH</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="K14">
+      <c r="E14" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K14" t="n">
         <v>9</v>
       </c>
       <c r="L14" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q14">
+        <v>144</v>
+      </c>
+      <c r="Q14" t="n">
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="str">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10" t="str">
         <f>Regions!M3</f>
         <v>IE-OY</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="K15">
+      <c r="E15" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15" t="s">
+        <v>164</v>
+      </c>
+      <c r="K15" t="n">
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q15">
+        <v>145</v>
+      </c>
+      <c r="Q15" t="n">
         <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="str">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10" t="str">
         <f>Regions!N3</f>
         <v>IE-WH</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="K16">
+      <c r="E16" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16" t="s">
+        <v>165</v>
+      </c>
+      <c r="K16" t="n">
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q16">
+        <v>146</v>
+      </c>
+      <c r="Q16" t="n">
         <v>11</v>
       </c>
       <c r="R16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8" t="str">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="str">
         <f>Regions!O3</f>
         <v>IE-WX</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="Q17">
+      <c r="E17" s="9"/>
+      <c r="F17"/>
+      <c r="G17" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q17" t="n">
         <v>12</v>
       </c>
       <c r="R17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8" t="str">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="str">
         <f>Regions!P3</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q18">
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q18" t="n">
         <v>13</v>
       </c>
       <c r="R18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8" t="str">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10" t="str">
         <f>Regions!Q3</f>
         <v>IE-CE</v>
       </c>
-      <c r="Q19">
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q19" t="n">
         <v>14</v>
       </c>
       <c r="R19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="C20" s="8" t="str">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9"/>
+      <c r="C20" s="10" t="str">
         <f>Regions!R3</f>
         <v>IE-CO</v>
       </c>
-      <c r="Q20">
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q20" t="n">
         <v>15</v>
       </c>
       <c r="R20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="C21" s="8" t="str">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9"/>
+      <c r="C21" s="10" t="str">
         <f>Regions!S3</f>
         <v>IE-KY</v>
       </c>
-      <c r="Q21">
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q21" t="n">
         <v>16</v>
       </c>
       <c r="R21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="C22" s="8" t="str">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9"/>
+      <c r="C22" s="10" t="str">
         <f>Regions!T3</f>
         <v>IE-LK</v>
       </c>
-      <c r="Q22">
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q22" t="n">
         <v>17</v>
       </c>
       <c r="R22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="C23" s="8" t="str">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9"/>
+      <c r="C23" s="10" t="str">
         <f>Regions!U3</f>
         <v>IE-TA</v>
       </c>
-      <c r="Q23">
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q23" t="n">
         <v>18</v>
       </c>
       <c r="R23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="C24" s="8" t="str">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9"/>
+      <c r="C24" s="10" t="str">
         <f>Regions!V3</f>
         <v>IE-WD</v>
       </c>
-      <c r="Q24">
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q24" t="n">
         <v>19</v>
       </c>
       <c r="R24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="C25" s="8" t="str">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9"/>
+      <c r="C25" s="10" t="str">
         <f>Regions!W3</f>
         <v>IE-G</v>
       </c>
-      <c r="Q25">
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q25" t="n">
         <v>20</v>
       </c>
       <c r="R25" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="C26" s="8" t="str">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9"/>
+      <c r="C26" s="10" t="str">
         <f>Regions!X3</f>
         <v>IE-LM</v>
       </c>
-      <c r="Q26">
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q26" t="n">
         <v>21</v>
       </c>
       <c r="R26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="C27" s="8" t="str">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9"/>
+      <c r="C27" s="10" t="str">
         <f>Regions!Y3</f>
         <v>IE-MO</v>
       </c>
-      <c r="Q27">
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q27" t="n">
         <v>22</v>
       </c>
       <c r="R27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="C28" s="8" t="str">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="9"/>
+      <c r="C28" s="10" t="str">
         <f>Regions!Z3</f>
         <v>IE-RN</v>
       </c>
-      <c r="Q28">
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q28" t="n">
         <v>23</v>
       </c>
       <c r="R28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="C29" s="8" t="str">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9"/>
+      <c r="C29" s="10" t="str">
         <f>Regions!AA3</f>
         <v>IE-SO</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="C30" s="8" t="str">
+    <row r="30">
+      <c r="A30" s="9"/>
+      <c r="C30" s="10" t="str">
         <f>Regions!AB3</f>
         <v>IE-CN</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="C31" s="8" t="str">
+    <row r="31">
+      <c r="A31" s="9"/>
+      <c r="C31" s="10" t="str">
         <f>Regions!AC3</f>
         <v>IE-DL</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="C32" s="8" t="str">
+    <row r="32">
+      <c r="A32" s="9"/>
+      <c r="C32" s="10" t="str">
         <f>Regions!AD3</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="8"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
+    <row r="33">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="9"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="10"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="9"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="9"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="9"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4">
+    <row r="4">
+      <c r="B4" t="n">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="14" t="s">
         <v>67</v>
       </c>
@@ -4947,117 +5149,117 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="13">
+    <row r="13">
+      <c r="B13" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="13">
+    <row r="14">
+      <c r="B14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="13">
+    <row r="15">
+      <c r="B15" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="13">
+    <row r="16">
+      <c r="B16" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="13">
+    <row r="17">
+      <c r="B17" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="13">
+    <row r="18">
+      <c r="B18" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
+    <row r="19">
+      <c r="B19" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
+    <row r="20">
+      <c r="B20" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
+    <row r="21">
+      <c r="B21" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="13">
+    <row r="22">
+      <c r="B22" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="13">
+    <row r="23">
+      <c r="B23" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="13">
+    <row r="24">
+      <c r="B24" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="B25" s="13"/>
-      <c r="C25" s="13">
+      <c r="C25" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="B26" s="13"/>
-      <c r="C26" s="13">
+      <c r="C26" s="13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="B27" s="13"/>
-      <c r="C27" s="13">
+      <c r="C27" s="13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5069,24 +5271,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B3:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
@@ -5094,43 +5296,43 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="B5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="19" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="13" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="B9" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5142,49 +5344,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="24"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2">
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3">
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -5202,7 +5404,7 @@
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5220,7 +5422,7 @@
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -5238,7 +5440,7 @@
       <c r="O10" s="26"/>
       <c r="P10" s="26"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -5256,7 +5458,7 @@
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -5274,7 +5476,7 @@
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="18.75" customHeight="1">
       <c r="A13" s="20" t="s">
         <v>56</v>
       </c>
@@ -5293,7 +5495,7 @@
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="25" t="s">
         <v>0</v>
       </c>
@@ -5313,7 +5515,7 @@
       <c r="O14" s="26"/>
       <c r="P14" s="26"/>
     </row>
-    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
@@ -5363,7 +5565,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26" t="s">
@@ -5371,7 +5573,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="26">
+      <c r="F16" s="26" t="n">
         <v>2222</v>
       </c>
       <c r="G16" s="26"/>
@@ -5389,7 +5591,7 @@
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26" t="s">
@@ -5397,7 +5599,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="26">
+      <c r="F17" s="26" t="n">
         <v>8888</v>
       </c>
       <c r="G17" s="26"/>
@@ -5415,7 +5617,7 @@
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -5433,7 +5635,7 @@
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -5451,7 +5653,7 @@
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -5469,7 +5671,7 @@
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -5487,7 +5689,7 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -5505,7 +5707,7 @@
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -5523,7 +5725,7 @@
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -5549,62 +5751,62 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="14" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="B1" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
+    <row r="3">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D5" s="7" t="s">
+    <row r="5">
+      <c r="D5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="9" t="n">
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28" t="s">
@@ -5612,11 +5814,11 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
-      <c r="G6" s="28">
+      <c r="G6" s="28" t="n">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
@@ -5629,344 +5831,344 @@
       <c r="F7" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="29" t="n">
         <f>CPI!$D$21/CPI!D3</f>
         <v>1.3926669328933141</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="str">
+    <row r="8">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B4,2))</f>
         <v>EUR01</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="27" t="n">
         <f>CPI!$D$21/CPI!D4</f>
         <v>1.3626878012654737</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="str">
+    <row r="9">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B5,2))</f>
         <v>EUR02</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="27" t="n">
         <f>CPI!$D$21/CPI!D5</f>
         <v>1.3346599424735295</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="str">
+    <row r="10">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B6,2))</f>
         <v>EUR03</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="27" t="n">
         <f>CPI!$D$21/CPI!D6</f>
         <v>1.3084901396799309</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="str">
+    <row r="11">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B7,2))</f>
         <v>EUR04</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="27" t="n">
         <f>CPI!$D$21/CPI!D7</f>
         <v>1.2828334702744419</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="str">
+    <row r="12">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B8,2))</f>
         <v>EUR05</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="27" t="n">
         <f>CPI!$D$21/CPI!D8</f>
         <v>1.2552186597597279</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="str">
+    <row r="13">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B9,2))</f>
         <v>EUR06</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="27" t="n">
         <f>CPI!$D$21/CPI!D9</f>
         <v>1.2281982972208687</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="str">
+    <row r="14">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B10,2))</f>
         <v>EUR07</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="27" t="n">
         <f>CPI!$D$21/CPI!D10</f>
         <v>1.2005848457682002</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="str">
+    <row r="15">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B11,2))</f>
         <v>EUR08</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="27" t="n">
         <f>CPI!$D$21/CPI!D11</f>
         <v>1.1577481637108971</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="str">
+    <row r="16">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B12,2))</f>
         <v>EUR09</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="27" t="n">
         <f>CPI!$D$21/CPI!D12</f>
         <v>1.1462853106048485</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7" t="str">
+    <row r="17">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B13,2))</f>
         <v>EUR10</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="27" t="n">
         <f>CPI!$D$21/CPI!D13</f>
         <v>1.1227084335013209</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7" t="str">
+    <row r="18">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B14,2))</f>
         <v>EUR11</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="27" t="n">
         <f>CPI!$D$21/CPI!D14</f>
         <v>1.0889509539295061</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="str">
+    <row r="19">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B15,2))</f>
         <v>EUR12</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="27" t="n">
         <f>CPI!$D$21/CPI!D15</f>
         <v>1.0613557055843141</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="str">
+    <row r="20">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B16,2))</f>
         <v>EUR13</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="27" t="n">
         <f>CPI!$D$21/CPI!D16</f>
         <v>1.045670645895876</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="str">
+    <row r="21">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B17,2))</f>
         <v>EUR14</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="27" t="n">
         <f>CPI!$D$21/CPI!D17</f>
         <v>1.0394340416460002</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7" t="str">
+    <row r="22">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B18,2))</f>
         <v>EUR15</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="27" t="n">
         <f>CPI!$D$21/CPI!D18</f>
         <v>1.0383956459999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7" t="str">
+    <row r="23">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B19,2))</f>
         <v>EUR16</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="27" t="n">
         <f>CPI!$D$21/CPI!D19</f>
         <v>1.0363230000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7" t="str">
+    <row r="24">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B20,2))</f>
         <v>EUR17</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="27" t="n">
         <f>CPI!$D$21/CPI!D20</f>
         <v>1.0190000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7" t="s">
+    <row r="25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="27" t="n">
         <f>CPI!$D$21/CPI!D22</f>
         <v>0.98522167487684731</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="9"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34">
       <c r="B34" s="27"/>
     </row>
   </sheetData>
@@ -5977,215 +6179,215 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+    <row r="2">
+      <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="B3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
+    <row r="4">
+      <c r="B4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="str">
+    <row r="5">
+      <c r="B5" s="9" t="str">
         <f>Constants!C7</f>
         <v>EUR00</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="str">
+    <row r="6">
+      <c r="B6" s="9" t="str">
         <f>Constants!C8</f>
         <v>EUR01</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="str">
+    <row r="7">
+      <c r="B7" s="9" t="str">
         <f>Constants!C9</f>
         <v>EUR02</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="str">
+    <row r="8">
+      <c r="B8" s="9" t="str">
         <f>Constants!C10</f>
         <v>EUR03</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="str">
+    <row r="9">
+      <c r="B9" s="9" t="str">
         <f>Constants!C11</f>
         <v>EUR04</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="str">
+    <row r="10">
+      <c r="B10" s="9" t="str">
         <f>Constants!C12</f>
         <v>EUR05</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="str">
+    <row r="11">
+      <c r="B11" s="9" t="str">
         <f>Constants!C13</f>
         <v>EUR06</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="str">
+    <row r="12">
+      <c r="B12" s="9" t="str">
         <f>Constants!C14</f>
         <v>EUR07</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="str">
+    <row r="13">
+      <c r="B13" s="9" t="str">
         <f>Constants!C15</f>
         <v>EUR08</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="str">
+    <row r="14">
+      <c r="B14" s="9" t="str">
         <f>Constants!C16</f>
         <v>EUR09</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="str">
+    <row r="15">
+      <c r="B15" s="9" t="str">
         <f>Constants!C17</f>
         <v>EUR10</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="str">
+    <row r="16">
+      <c r="B16" s="9" t="str">
         <f>Constants!C18</f>
         <v>EUR11</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="str">
+    <row r="17">
+      <c r="B17" s="9" t="str">
         <f>Constants!C19</f>
         <v>EUR12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="str">
+    <row r="18">
+      <c r="B18" s="9" t="str">
         <f>Constants!C20</f>
         <v>EUR13</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="str">
+    <row r="19">
+      <c r="B19" s="9" t="str">
         <f>Constants!C21</f>
         <v>EUR14</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="str">
+    <row r="20">
+      <c r="B20" s="9" t="str">
         <f>Constants!C22</f>
         <v>EUR15</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="str">
+    <row r="21">
+      <c r="B21" s="9" t="str">
         <f>Constants!C23</f>
         <v>EUR16</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="7" t="str">
+    <row r="22">
+      <c r="B22" s="9" t="str">
         <f>Constants!C24</f>
         <v>EUR17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="str">
+    <row r="23">
+      <c r="B23" s="9" t="str">
         <f>Constants!C25</f>
         <v>EUR19</v>
       </c>
@@ -6198,20 +6400,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B2:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="30" customHeight="1">
       <c r="B2" s="30"/>
       <c r="C2" s="31" t="s">
         <v>38</v>
@@ -6220,244 +6423,244 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="33">
+    <row r="3" ht="15" customHeight="1">
+      <c r="B3" s="33" t="n">
         <v>2000</v>
       </c>
       <c r="C3" s="34"/>
-      <c r="D3" s="34">
+      <c r="D3" s="34" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="33">
+    <row r="4" ht="15" customHeight="1">
+      <c r="B4" s="33" t="n">
         <v>2001</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="34" t="n">
         <f t="shared" ref="D4:D22" si="0">D3+D3*C4</f>
         <v>102.2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="33">
+    <row r="5" ht="15" customHeight="1">
+      <c r="B5" s="33" t="n">
         <v>2002</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="35" t="n">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="36" t="n">
         <f t="shared" si="0"/>
         <v>104.34620000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="33">
+    <row r="6" ht="15" customHeight="1">
+      <c r="B6" s="33" t="n">
         <v>2003</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="35" t="n">
         <v>0.02</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="36" t="n">
         <f t="shared" si="0"/>
         <v>106.43312400000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="33">
+    <row r="7" ht="15" customHeight="1">
+      <c r="B7" s="33" t="n">
         <v>2004</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="35" t="n">
         <v>0.02</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="36" t="n">
         <f t="shared" si="0"/>
         <v>108.56178648000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="33">
+    <row r="8" ht="15" customHeight="1">
+      <c r="B8" s="33" t="n">
         <v>2005</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="36" t="n">
         <f t="shared" si="0"/>
         <v>110.95014578256001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="33">
+    <row r="9" ht="15" customHeight="1">
+      <c r="B9" s="33" t="n">
         <v>2006</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="36" t="n">
         <f t="shared" si="0"/>
         <v>113.39104898977634</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="33">
+    <row r="10" ht="15" customHeight="1">
+      <c r="B10" s="33" t="n">
         <v>2007</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="35" t="n">
         <v>2.3E-2</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="36" t="n">
         <f t="shared" si="0"/>
         <v>115.99904311654119</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="33">
+    <row r="11" ht="15" customHeight="1">
+      <c r="B11" s="33" t="n">
         <v>2008</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="35" t="n">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="36" t="n">
         <f t="shared" si="0"/>
         <v>120.29100771185321</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="33">
+    <row r="12" ht="15" customHeight="1">
+      <c r="B12" s="33" t="n">
         <v>2009</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="35" t="n">
         <v>0.01</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="36" t="n">
         <f t="shared" si="0"/>
         <v>121.49391778897174</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="33">
+    <row r="13" ht="15" customHeight="1">
+      <c r="B13" s="33" t="n">
         <v>2010</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="35" t="n">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="36" t="n">
         <f t="shared" si="0"/>
         <v>124.04529006254015</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="33">
+    <row r="14" ht="15" customHeight="1">
+      <c r="B14" s="33" t="n">
         <v>2011</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="35" t="n">
         <v>3.1E-2</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="36" t="n">
         <f t="shared" si="0"/>
         <v>127.89069405447889</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="33">
+    <row r="15" ht="15" customHeight="1">
+      <c r="B15" s="33" t="n">
         <v>2012</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="35" t="n">
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="36" t="n">
         <f t="shared" si="0"/>
         <v>131.21585209989533</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="33">
+    <row r="16" ht="15" customHeight="1">
+      <c r="B16" s="33" t="n">
         <v>2013</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="35" t="n">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="36" t="n">
         <f t="shared" si="0"/>
         <v>133.18408988139376</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="33">
+    <row r="17" ht="15" customHeight="1">
+      <c r="B17" s="33" t="n">
         <v>2014</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="35" t="n">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="36" t="n">
         <f t="shared" si="0"/>
         <v>133.98319442068211</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="33">
+    <row r="18" ht="15" customHeight="1">
+      <c r="B18" s="33" t="n">
         <v>2015</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="41" t="n">
         <v>1E-3</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="36" t="n">
         <f>D17+D17*C18</f>
         <v>134.1171776151028</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="38">
+    <row r="19" ht="15" customHeight="1">
+      <c r="B19" s="38" t="n">
         <v>2016</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="39" t="n">
         <v>2E-3</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="40" t="n">
         <f t="shared" si="0"/>
         <v>134.385411970333</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="38">
+    <row r="20" ht="15" customHeight="1">
+      <c r="B20" s="38" t="n">
         <v>2017</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="39" t="n">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="40" t="n">
         <f t="shared" si="0"/>
         <v>136.66996397382866</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
+    <row r="21" ht="15" customHeight="1">
+      <c r="B21" s="38" t="n">
         <v>2018</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="39" t="n">
         <v>1.9E-2</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="40" t="n">
         <f t="shared" si="0"/>
         <v>139.26669328933141</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="38">
+    <row r="22" ht="15" customHeight="1">
+      <c r="B22" s="38" t="n">
         <v>2019</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="39" t="n">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="40" t="n">
         <f t="shared" si="0"/>
         <v>141.35569368867138</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" ht="15" customHeight="1">
       <c r="B24" s="37" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Add a CG to remove domain violations in IND SubRES
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9938C528-DEA8-4E8C-BF72-13CE42EE050F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CB742D-73A0-477C-B144-2EA5C1861533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Constants" sheetId="25" r:id="rId6"/>
     <sheet name="Defaults" sheetId="26" r:id="rId7"/>
     <sheet name="CPI" sheetId="23" r:id="rId8"/>
+    <sheet name="temp_cg" sheetId="28" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="143">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -472,6 +473,30 @@
   </si>
   <si>
     <t>Hour</t>
+  </si>
+  <si>
+    <t>~TFM_COMGRP</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>IIS_Gases</t>
+  </si>
+  <si>
+    <t>IIS CommGrp for gases</t>
+  </si>
+  <si>
+    <t>INDGAS, INDIIS, INDCOG, INDCOP</t>
+  </si>
+  <si>
+    <t>Allregions</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -952,7 +977,7 @@
                   <a14:compatExt spid="_x0000_s8193"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14BED322-D23C-467E-B772-BF4CD143C40D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1374,7 +1399,7 @@
         <xdr:cNvPr id="2050" name="Text Box 1026" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19F9368B-7ACB-45A2-9F2F-09CB5F1E82C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,7 +1458,7 @@
         <xdr:cNvPr id="2052" name="Text Box 1028" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E058AC4-72D7-4345-A791-95CC6C0BB5D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1492,7 +1517,7 @@
         <xdr:cNvPr id="2053" name="Text Box 1029" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33F89FC-6BFE-4F14-8830-38504D114B69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1551,7 +1576,7 @@
         <xdr:cNvPr id="2055" name="Text Box 1031" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E87EF87-62DE-4365-A04D-D4C872A6466F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1610,7 +1635,7 @@
         <xdr:cNvPr id="2056" name="Text Box 1032" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1078967B-24C9-4029-ACB0-E2DAEAF287F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1669,7 +1694,7 @@
         <xdr:cNvPr id="2057" name="Text Box 1033" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19ED809E-E0A2-409D-B948-8FCA1E4546DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1728,7 +1753,7 @@
         <xdr:cNvPr id="2058" name="Text Box 1034" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A5DE7E3-549D-4985-859C-9AB51B27AFE5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1787,7 +1812,7 @@
         <xdr:cNvPr id="2059" name="Text Box 1035" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFE2BD73-5422-4F1B-AFC6-5C1DAB6637C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4302,7 +4327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
@@ -6202,7 +6227,7 @@
   <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6466,4 +6491,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85124094-EF73-46AF-B3F7-671AC3531E13}">
+  <dimension ref="B3:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add yearly time-period in System Setting
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CB742D-73A0-477C-B144-2EA5C1861533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28A59F0-1AAF-401A-ADCE-AAE8D9178084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="144">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -498,6 +498,9 @@
   <si>
     <t>Y</t>
   </si>
+  <si>
+    <t>P32</t>
+  </si>
 </sst>
 </file>
 
@@ -506,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -515,6 +518,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -628,6 +632,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -965,7 +974,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>30480</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1860,16 +1869,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>421005</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>48577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>402909</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>509589</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>10478</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1884,8 +1893,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4252913" y="395287"/>
-          <a:ext cx="6927534" cy="1924051"/>
+          <a:off x="5937885" y="551497"/>
+          <a:ext cx="7967664" cy="1973581"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3650,38 +3659,38 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" customWidth="1"/>
+    <col min="16" max="16" width="7.109375" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1"/>
+    <col min="19" max="19" width="5.88671875" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" customWidth="1"/>
     <col min="23" max="23" width="5" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" customWidth="1"/>
     <col min="26" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="str">
         <f t="array" ref="C3">IF(INDEX(C5:C7,$A$4)&lt;&gt;0,INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -3795,13 +3804,13 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3916,7 +3925,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3952,7 +3961,7 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -4066,7 +4075,7 @@
       </c>
       <c r="AD7" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -4074,7 +4083,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>76</v>
       </c>
@@ -4082,7 +4091,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>78</v>
       </c>
@@ -4090,7 +4099,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>80</v>
       </c>
@@ -4098,7 +4107,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>82</v>
       </c>
@@ -4106,7 +4115,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>84</v>
       </c>
@@ -4114,7 +4123,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -4122,7 +4131,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
@@ -4130,7 +4139,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
@@ -4138,7 +4147,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>92</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>94</v>
       </c>
@@ -4154,7 +4163,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>96</v>
       </c>
@@ -4162,7 +4171,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>98</v>
       </c>
@@ -4170,7 +4179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
@@ -4178,7 +4187,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>102</v>
       </c>
@@ -4186,7 +4195,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>104</v>
       </c>
@@ -4194,7 +4203,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>106</v>
       </c>
@@ -4202,7 +4211,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>108</v>
       </c>
@@ -4210,7 +4219,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>110</v>
       </c>
@@ -4218,7 +4227,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>112</v>
       </c>
@@ -4226,7 +4235,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>114</v>
       </c>
@@ -4234,7 +4243,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>116</v>
       </c>
@@ -4242,7 +4251,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>118</v>
       </c>
@@ -4250,7 +4259,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>120</v>
       </c>
@@ -4258,7 +4267,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>122</v>
       </c>
@@ -4266,7 +4275,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>124</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>126</v>
       </c>
@@ -4282,7 +4291,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>128</v>
       </c>
@@ -4308,7 +4317,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>30480</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -4331,16 +4340,16 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="2.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="11" t="s">
         <v>6</v>
@@ -4351,7 +4360,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="9" t="s">
         <v>12</v>
@@ -4387,7 +4396,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>37</v>
@@ -4424,7 +4433,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="str">
@@ -4453,7 +4462,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="str">
@@ -4482,7 +4491,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="str">
@@ -4511,7 +4520,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="str">
@@ -4537,7 +4546,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="str">
@@ -4563,7 +4572,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="str">
@@ -4590,7 +4599,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="str">
@@ -4611,7 +4620,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="str">
@@ -4632,7 +4641,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="str">
@@ -4653,7 +4662,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="str">
@@ -4674,7 +4683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="str">
@@ -4695,7 +4704,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="str">
@@ -4710,7 +4719,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="str">
@@ -4724,7 +4733,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="str">
@@ -4738,7 +4747,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="str">
         <f>Regions!R3</f>
@@ -4751,7 +4760,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="str">
         <f>Regions!S3</f>
@@ -4764,7 +4773,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="str">
         <f>Regions!T3</f>
@@ -4777,7 +4786,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="str">
         <f>Regions!U3</f>
@@ -4790,7 +4799,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="str">
         <f>Regions!V3</f>
@@ -4803,7 +4812,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="str">
         <f>Regions!W3</f>
@@ -4816,7 +4825,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="str">
         <f>Regions!X3</f>
@@ -4829,7 +4838,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="str">
         <f>Regions!Y3</f>
@@ -4842,7 +4851,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="C28" s="8" t="str">
         <f>Regions!Z3</f>
@@ -4855,38 +4864,38 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="C29" s="8" t="str">
         <f>Regions!AA3</f>
         <v>IE-SO</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="C30" s="8" t="str">
         <f>Regions!AB3</f>
         <v>IE-CN</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="C31" s="8" t="str">
         <f>Regions!AC3</f>
         <v>IE-DL</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="C32" s="8" t="str">
         <f>Regions!AD3</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
@@ -4895,19 +4904,19 @@
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
     </row>
   </sheetData>
@@ -4924,169 +4933,303 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:C27"/>
+  <dimension ref="B3:D44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="13">
         <v>4</v>
       </c>
       <c r="C14" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="13">
         <v>5</v>
       </c>
       <c r="C15" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
         <v>5</v>
       </c>
       <c r="C16" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
         <v>5</v>
       </c>
       <c r="C17" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <v>5</v>
       </c>
       <c r="C18" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
         <v>5</v>
       </c>
       <c r="C19" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
         <v>5</v>
       </c>
       <c r="C20" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="13">
         <v>5</v>
       </c>
       <c r="C21" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="13">
         <v>5</v>
       </c>
       <c r="C22" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="13">
         <v>5</v>
       </c>
       <c r="C23" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="13">
         <v>5</v>
       </c>
       <c r="C24" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="13"/>
       <c r="C25" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="13"/>
       <c r="C26" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="13"/>
       <c r="C27" s="13">
         <v>5</v>
       </c>
+      <c r="D27" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="13">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
@@ -5101,17 +5244,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
@@ -5119,7 +5262,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>31</v>
       </c>
@@ -5127,7 +5270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>32</v>
       </c>
@@ -5135,7 +5278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>33</v>
       </c>
@@ -5143,7 +5286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>34</v>
       </c>
@@ -5151,7 +5294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>53</v>
       </c>
@@ -5174,42 +5317,42 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -5227,7 +5370,7 @@
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5245,7 +5388,7 @@
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -5263,7 +5406,7 @@
       <c r="O10" s="26"/>
       <c r="P10" s="26"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -5281,7 +5424,7 @@
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -5299,7 +5442,7 @@
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
         <v>56</v>
       </c>
@@ -5318,7 +5461,7 @@
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>0</v>
       </c>
@@ -5338,7 +5481,7 @@
       <c r="O14" s="26"/>
       <c r="P14" s="26"/>
     </row>
-    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
@@ -5388,7 +5531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26" t="s">
@@ -5414,7 +5557,7 @@
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26" t="s">
@@ -5440,7 +5583,7 @@
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -5458,7 +5601,7 @@
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -5476,7 +5619,7 @@
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -5494,7 +5637,7 @@
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -5512,7 +5655,7 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -5530,7 +5673,7 @@
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -5548,7 +5691,7 @@
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -5581,27 +5724,27 @@
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
@@ -5621,7 +5764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
@@ -5629,7 +5772,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28" t="s">
@@ -5641,7 +5784,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
@@ -5659,7 +5802,7 @@
         <v>1.3926669328933141</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B4,2))</f>
@@ -5677,7 +5820,7 @@
         <v>1.3626878012654737</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B5,2))</f>
@@ -5695,7 +5838,7 @@
         <v>1.3346599424735295</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B6,2))</f>
@@ -5713,7 +5856,7 @@
         <v>1.3084901396799309</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B7,2))</f>
@@ -5731,7 +5874,7 @@
         <v>1.2828334702744419</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B8,2))</f>
@@ -5749,7 +5892,7 @@
         <v>1.2552186597597279</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B9,2))</f>
@@ -5767,7 +5910,7 @@
         <v>1.2281982972208687</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B10,2))</f>
@@ -5785,7 +5928,7 @@
         <v>1.2005848457682002</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B11,2))</f>
@@ -5803,7 +5946,7 @@
         <v>1.1577481637108971</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B12,2))</f>
@@ -5821,7 +5964,7 @@
         <v>1.1462853106048485</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B13,2))</f>
@@ -5839,7 +5982,7 @@
         <v>1.1227084335013209</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B14,2))</f>
@@ -5857,7 +6000,7 @@
         <v>1.0889509539295061</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B15,2))</f>
@@ -5875,7 +6018,7 @@
         <v>1.0613557055843141</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B16,2))</f>
@@ -5893,7 +6036,7 @@
         <v>1.045670645895876</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B17,2))</f>
@@ -5911,7 +6054,7 @@
         <v>1.0394340416460002</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B18,2))</f>
@@ -5929,7 +6072,7 @@
         <v>1.0383956459999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B19,2))</f>
@@ -5947,7 +6090,7 @@
         <v>1.0363230000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B20,2))</f>
@@ -5965,7 +6108,7 @@
         <v>1.0190000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>69</v>
@@ -5982,16 +6125,16 @@
         <v>0.98522167487684731</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B34" s="27"/>
     </row>
   </sheetData>
@@ -6009,12 +6152,12 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
@@ -6022,7 +6165,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>48</v>
       </c>
@@ -6051,7 +6194,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>68</v>
       </c>
@@ -6071,7 +6214,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="str">
         <f>Constants!C7</f>
         <v>EUR00</v>
@@ -6092,7 +6235,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="str">
         <f>Constants!C8</f>
         <v>EUR01</v>
@@ -6113,103 +6256,103 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="str">
         <f>Constants!C9</f>
         <v>EUR02</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="str">
         <f>Constants!C10</f>
         <v>EUR03</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="str">
         <f>Constants!C11</f>
         <v>EUR04</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="str">
         <f>Constants!C12</f>
         <v>EUR05</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="str">
         <f>Constants!C13</f>
         <v>EUR06</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="str">
         <f>Constants!C14</f>
         <v>EUR07</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="str">
         <f>Constants!C15</f>
         <v>EUR08</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="str">
         <f>Constants!C16</f>
         <v>EUR09</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="str">
         <f>Constants!C17</f>
         <v>EUR10</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="str">
         <f>Constants!C18</f>
         <v>EUR11</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="str">
         <f>Constants!C19</f>
         <v>EUR12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="str">
         <f>Constants!C20</f>
         <v>EUR13</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="str">
         <f>Constants!C21</f>
         <v>EUR14</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="str">
         <f>Constants!C22</f>
         <v>EUR15</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="str">
         <f>Constants!C23</f>
         <v>EUR16</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="str">
         <f>Constants!C24</f>
         <v>EUR17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="str">
         <f>Constants!C25</f>
         <v>EUR19</v>
@@ -6230,13 +6373,13 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="4" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="30"/>
       <c r="C2" s="31" t="s">
         <v>38</v>
@@ -6245,7 +6388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B3" s="33">
         <v>2000</v>
       </c>
@@ -6254,7 +6397,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B4" s="33">
         <v>2001</v>
       </c>
@@ -6266,7 +6409,7 @@
         <v>102.2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B5" s="33">
         <v>2002</v>
       </c>
@@ -6278,7 +6421,7 @@
         <v>104.34620000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B6" s="33">
         <v>2003</v>
       </c>
@@ -6290,7 +6433,7 @@
         <v>106.43312400000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B7" s="33">
         <v>2004</v>
       </c>
@@ -6302,7 +6445,7 @@
         <v>108.56178648000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B8" s="33">
         <v>2005</v>
       </c>
@@ -6314,7 +6457,7 @@
         <v>110.95014578256001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B9" s="33">
         <v>2006</v>
       </c>
@@ -6326,7 +6469,7 @@
         <v>113.39104898977634</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B10" s="33">
         <v>2007</v>
       </c>
@@ -6338,7 +6481,7 @@
         <v>115.99904311654119</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B11" s="33">
         <v>2008</v>
       </c>
@@ -6350,7 +6493,7 @@
         <v>120.29100771185321</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B12" s="33">
         <v>2009</v>
       </c>
@@ -6362,7 +6505,7 @@
         <v>121.49391778897174</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B13" s="33">
         <v>2010</v>
       </c>
@@ -6374,7 +6517,7 @@
         <v>124.04529006254015</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B14" s="33">
         <v>2011</v>
       </c>
@@ -6386,7 +6529,7 @@
         <v>127.89069405447889</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B15" s="33">
         <v>2012</v>
       </c>
@@ -6398,7 +6541,7 @@
         <v>131.21585209989533</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B16" s="33">
         <v>2013</v>
       </c>
@@ -6410,7 +6553,7 @@
         <v>133.18408988139376</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B17" s="33">
         <v>2014</v>
       </c>
@@ -6422,7 +6565,7 @@
         <v>133.98319442068211</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B18" s="33">
         <v>2015</v>
       </c>
@@ -6434,7 +6577,7 @@
         <v>134.1171776151028</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <v>2016</v>
       </c>
@@ -6446,7 +6589,7 @@
         <v>134.385411970333</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B20" s="38">
         <v>2017</v>
       </c>
@@ -6458,7 +6601,7 @@
         <v>136.66996397382866</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B21" s="38">
         <v>2018</v>
       </c>
@@ -6470,7 +6613,7 @@
         <v>139.26669328933141</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B22" s="38">
         <v>2019</v>
       </c>
@@ -6482,7 +6625,7 @@
         <v>141.35569368867138</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
         <v>40</v>
       </c>
@@ -6497,23 +6640,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85124094-EF73-46AF-B3F7-671AC3531E13}">
   <dimension ref="B3:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>136</v>
       </c>
@@ -6527,7 +6670,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Add yearly time period in Sys. Setting file
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28A59F0-1AAF-401A-ADCE-AAE8D9178084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBC4F2B-653B-4663-9F5B-D1E2ED342DED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t>P32</t>
+    <t>P33</t>
   </si>
 </sst>
 </file>
@@ -4933,10 +4933,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:D44"/>
+  <dimension ref="B3:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5225,6 +5225,11 @@
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="13">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Kt, PJ and MEuro units
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA6DBC9-BE41-4BC5-A256-C86C2E91AC94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC340E9-40C0-49C1-9284-E1B3B645315F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="158">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -6051,7 +6051,7 @@
   <dimension ref="B2:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6292,17 +6292,44 @@
         <f>Constants!C15</f>
         <v>EUR08</v>
       </c>
+      <c r="N13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="str">
         <f>Constants!C16</f>
         <v>EUR09</v>
       </c>
+      <c r="N14" t="s">
+        <v>149</v>
+      </c>
+      <c r="O14" t="s">
+        <v>149</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="str">
         <f>Constants!C17</f>
         <v>EUR10</v>
+      </c>
+      <c r="N15" t="s">
+        <v>157</v>
+      </c>
+      <c r="O15" t="s">
+        <v>157</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Data centre demand add
Transport demand covid adjusted
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GDrive\PhD\Veda_2\IrishTimes_GIT\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1201B8-9DAB-4815-88EB-B424FAEEA2F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAE37E6-3FE9-443A-A620-42B0AE23D367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="4230" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="10080" windowHeight="7875" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -34,18 +34,7 @@
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -554,7 +543,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -679,6 +668,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -736,7 +731,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -853,11 +848,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -874,8 +880,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -926,7 +930,10 @@
     <xf numFmtId="10" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5014,10 +5021,10 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="41" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="42" t="s">
@@ -5025,258 +5032,294 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="13">
+      <c r="B13" s="43">
         <v>1</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="43">
         <v>1</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="13">
+      <c r="B14" s="43">
         <v>4</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="43">
         <v>1</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="13">
+      <c r="B15" s="43">
         <v>5</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="43">
         <v>1</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="13">
+      <c r="B16" s="43">
         <v>5</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="43">
         <v>1</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="13">
+      <c r="B17" s="43">
         <v>5</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="43">
         <v>1</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="13">
+      <c r="B18" s="43">
         <v>5</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="43">
         <v>5</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
+      <c r="B19" s="43">
         <v>5</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="43">
         <v>5</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
+      <c r="B20" s="43">
         <v>5</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="43">
         <v>5</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
+      <c r="B21" s="43">
         <v>5</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="43">
         <v>5</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="13">
+      <c r="B22" s="43">
         <v>5</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="43">
         <v>5</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="13">
+      <c r="B23" s="43">
         <v>5</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="43">
         <v>5</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="13">
+      <c r="B24" s="43">
         <v>5</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="43">
         <v>5</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13">
+      <c r="B25" s="43"/>
+      <c r="C25" s="43">
         <v>5</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13">
+      <c r="B26" s="43"/>
+      <c r="C26" s="43">
         <v>5</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="13"/>
-      <c r="C27" s="13">
+      <c r="B27" s="43"/>
+      <c r="C27" s="43">
         <v>5</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="19">
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="19">
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="19">
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="19">
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="19">
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" s="19">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" s="19">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="19">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" s="19">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="19">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" s="19">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="19">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="19">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="19">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="19">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D43" s="19">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D44" s="19">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D45" s="19">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5294,23 +5337,23 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
     </row>
@@ -5371,387 +5414,387 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
+      <c r="A1" s="22"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="O2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
     </row>
     <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="23" t="s">
+      <c r="N15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="23" t="s">
+      <c r="O15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="23" t="s">
+      <c r="P15" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26">
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24">
         <v>2222</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26">
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24">
         <v>8888</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26" t="s">
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5779,7 +5822,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>46</v>
       </c>
     </row>
@@ -5817,31 +5860,31 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28">
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26">
         <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="str">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
         <v>EUR00</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28" t="s">
+      <c r="E7" s="26"/>
+      <c r="F7" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="27">
         <f>CPI!$D$21/CPI!D3</f>
         <v>1.3926669328933141</v>
       </c>
@@ -5859,7 +5902,7 @@
       <c r="F8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="25">
         <f>CPI!$D$21/CPI!D4</f>
         <v>1.3626878012654737</v>
       </c>
@@ -5877,7 +5920,7 @@
       <c r="F9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="25">
         <f>CPI!$D$21/CPI!D5</f>
         <v>1.3346599424735295</v>
       </c>
@@ -5895,7 +5938,7 @@
       <c r="F10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="25">
         <f>CPI!$D$21/CPI!D6</f>
         <v>1.3084901396799309</v>
       </c>
@@ -5913,7 +5956,7 @@
       <c r="F11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="25">
         <f>CPI!$D$21/CPI!D7</f>
         <v>1.2828334702744419</v>
       </c>
@@ -5931,7 +5974,7 @@
       <c r="F12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="25">
         <f>CPI!$D$21/CPI!D8</f>
         <v>1.2552186597597279</v>
       </c>
@@ -5949,7 +5992,7 @@
       <c r="F13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="25">
         <f>CPI!$D$21/CPI!D9</f>
         <v>1.2281982972208687</v>
       </c>
@@ -5967,7 +6010,7 @@
       <c r="F14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="25">
         <f>CPI!$D$21/CPI!D10</f>
         <v>1.2005848457682002</v>
       </c>
@@ -5985,7 +6028,7 @@
       <c r="F15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="25">
         <f>CPI!$D$21/CPI!D11</f>
         <v>1.1577481637108971</v>
       </c>
@@ -6003,7 +6046,7 @@
       <c r="F16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="25">
         <f>CPI!$D$21/CPI!D12</f>
         <v>1.1462853106048485</v>
       </c>
@@ -6021,7 +6064,7 @@
       <c r="F17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="25">
         <f>CPI!$D$21/CPI!D13</f>
         <v>1.1227084335013209</v>
       </c>
@@ -6039,7 +6082,7 @@
       <c r="F18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="25">
         <f>CPI!$D$21/CPI!D14</f>
         <v>1.0889509539295061</v>
       </c>
@@ -6057,7 +6100,7 @@
       <c r="F19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="25">
         <f>CPI!$D$21/CPI!D15</f>
         <v>1.0613557055843141</v>
       </c>
@@ -6075,7 +6118,7 @@
       <c r="F20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="25">
         <f>CPI!$D$21/CPI!D16</f>
         <v>1.045670645895876</v>
       </c>
@@ -6093,7 +6136,7 @@
       <c r="F21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="25">
         <f>CPI!$D$21/CPI!D17</f>
         <v>1.0394340416460002</v>
       </c>
@@ -6111,7 +6154,7 @@
       <c r="F22" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="25">
         <f>CPI!$D$21/CPI!D18</f>
         <v>1.0383956459999999</v>
       </c>
@@ -6129,7 +6172,7 @@
       <c r="F23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="25">
         <f>CPI!$D$21/CPI!D19</f>
         <v>1.0363230000000001</v>
       </c>
@@ -6147,7 +6190,7 @@
       <c r="F24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="25">
         <f>CPI!$D$21/CPI!D20</f>
         <v>1.0190000000000001</v>
       </c>
@@ -6164,7 +6207,7 @@
       <c r="F25" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="25">
         <f>CPI!$D$21/CPI!D22</f>
         <v>0.98522167487684731</v>
       </c>
@@ -6179,7 +6222,7 @@
       <c r="B33" s="7"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
+      <c r="B34" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6544,253 +6587,253 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="33">
+      <c r="B3" s="31">
         <v>2000</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="33">
+      <c r="B4" s="31">
         <v>2001</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="33">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="32">
         <f t="shared" ref="D4:D22" si="0">D3+D3*C4</f>
         <v>102.2</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="33">
+      <c r="B5" s="31">
         <v>2002</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="33">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="34">
         <f t="shared" si="0"/>
         <v>104.34620000000001</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="33">
+      <c r="B6" s="31">
         <v>2003</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="33">
         <v>0.02</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="34">
         <f t="shared" si="0"/>
         <v>106.43312400000001</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="33">
+      <c r="B7" s="31">
         <v>2004</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="33">
         <v>0.02</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="34">
         <f t="shared" si="0"/>
         <v>108.56178648000001</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="33">
+      <c r="B8" s="31">
         <v>2005</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="33">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="34">
         <f t="shared" si="0"/>
         <v>110.95014578256001</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="33">
+      <c r="B9" s="31">
         <v>2006</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="33">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="34">
         <f t="shared" si="0"/>
         <v>113.39104898977634</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="33">
+      <c r="B10" s="31">
         <v>2007</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="33">
         <v>2.3E-2</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="34">
         <f t="shared" si="0"/>
         <v>115.99904311654119</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="33">
+      <c r="B11" s="31">
         <v>2008</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="33">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="34">
         <f t="shared" si="0"/>
         <v>120.29100771185321</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="33">
+      <c r="B12" s="31">
         <v>2009</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="33">
         <v>0.01</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="34">
         <f t="shared" si="0"/>
         <v>121.49391778897174</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="33">
+      <c r="B13" s="31">
         <v>2010</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="33">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="34">
         <f t="shared" si="0"/>
         <v>124.04529006254015</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="33">
+      <c r="B14" s="31">
         <v>2011</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="33">
         <v>3.1E-2</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="34">
         <f t="shared" si="0"/>
         <v>127.89069405447889</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="33">
+      <c r="B15" s="31">
         <v>2012</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="33">
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="34">
         <f t="shared" si="0"/>
         <v>131.21585209989533</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="33">
+      <c r="B16" s="31">
         <v>2013</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="33">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="34">
         <f t="shared" si="0"/>
         <v>133.18408988139376</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="33">
+      <c r="B17" s="31">
         <v>2014</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="34">
         <f t="shared" si="0"/>
         <v>133.98319442068211</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="33">
+      <c r="B18" s="31">
         <v>2015</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="39">
         <v>1E-3</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="34">
         <f>D17+D17*C18</f>
         <v>134.1171776151028</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="38">
+      <c r="B19" s="36">
         <v>2016</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="37">
         <v>2E-3</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="38">
         <f t="shared" si="0"/>
         <v>134.385411970333</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="38">
+      <c r="B20" s="36">
         <v>2017</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="37">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="38">
         <f t="shared" si="0"/>
         <v>136.66996397382866</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
+      <c r="B21" s="36">
         <v>2018</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="37">
         <v>1.9E-2</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="38">
         <f t="shared" si="0"/>
         <v>139.26669328933141</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="38">
+      <c r="B22" s="36">
         <v>2019</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="37">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="38">
         <f t="shared" si="0"/>
         <v>141.35569368867138</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="35" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change discount rate to 4% and discount year to 2018
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1201B8-9DAB-4815-88EB-B424FAEEA2F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E13076E-08FA-422B-8AF6-6176E8581E6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="4230" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -4975,7 +4975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -5764,8 +5764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5813,7 +5813,7 @@
         <v>43</v>
       </c>
       <c r="G5" s="7">
-        <v>2012</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
@@ -5825,7 +5825,7 @@
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change to 40 ts
- specify AFs for REN in PWR
- specify COM_FR for passenger demand in TRA
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E13076E-08FA-422B-8AF6-6176E8581E6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Regions" sheetId="27" r:id="rId1"/>
-    <sheet name="Region-Time Slices" sheetId="20" r:id="rId2"/>
-    <sheet name="TimePeriods" sheetId="24" r:id="rId3"/>
-    <sheet name="Import Settings" sheetId="17" r:id="rId4"/>
-    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId5"/>
-    <sheet name="Constants" sheetId="25" r:id="rId6"/>
-    <sheet name="Defaults" sheetId="26" r:id="rId7"/>
-    <sheet name="CPI" sheetId="23" r:id="rId8"/>
-    <sheet name="temp_cg" sheetId="28" r:id="rId9"/>
+    <sheet name="Regions" sheetId="27" state="visible" r:id="rId1"/>
+    <sheet name="Region-Time Slices" sheetId="20" state="visible" r:id="rId2"/>
+    <sheet name="TimePeriods" sheetId="24" state="visible" r:id="rId3"/>
+    <sheet name="Import Settings" sheetId="17" state="visible" r:id="rId4"/>
+    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" state="visible" r:id="rId5"/>
+    <sheet name="Constants" sheetId="25" state="visible" r:id="rId6"/>
+    <sheet name="Defaults" sheetId="26" state="visible" r:id="rId7"/>
+    <sheet name="CPI" sheetId="23" state="visible" r:id="rId8"/>
+    <sheet name="temp_cg" sheetId="28" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -35,22 +28,11 @@
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="175">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -546,15 +528,63 @@
   <si>
     <t>P33</t>
   </si>
+  <si>
+    <t xml:space="preserve">Wi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Su</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hour</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -565,119 +595,83 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <b/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
       <b/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="53"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="10">
@@ -745,24 +739,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -771,11 +758,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -790,7 +775,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -799,44 +783,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -851,88 +797,168 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -944,12 +970,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1065,7 +1087,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -1906,7 +1928,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -2303,7 +2325,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2480,7 +2502,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2702,7 +2724,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -3154,7 +3176,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -3342,31 +3364,31 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="season_info" displayName="season_info" ref="K4:L16" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="season_info" displayName="season_info" ref="K4:L16" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Month"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Season"/>
+    <tableColumn id="1" name="Month"/>
+    <tableColumn id="2" name="Season"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="weekly_info" displayName="weekly_info" ref="N4:O11" totalsRowShown="0">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="weekly_info" displayName="weekly_info" ref="N4:O11" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Day"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Type"/>
+    <tableColumn id="1" name="Day"/>
+    <tableColumn id="2" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="daynite_info" displayName="daynite_info" ref="Q4:R28" totalsRowShown="0">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="daynite_info" displayName="daynite_info" ref="Q4:R28" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
+    <tableColumn id="1" name="Hour"/>
+    <tableColumn id="2" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3692,45 +3714,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AD37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1"/>
-    <col min="23" max="23" width="5" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" customWidth="1"/>
-    <col min="26" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="5" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="6" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="18" max="18" width="6" hidden="0" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" hidden="0" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" hidden="0" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="23" max="23" width="5" hidden="0" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="6" hidden="0" customWidth="1"/>
+    <col min="27" max="27" width="6" hidden="0" customWidth="1"/>
+    <col min="28" max="28" width="6" hidden="0" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="15" customHeight="1">
       <c r="C3" s="2" t="str">
         <f t="array" ref="C3">IF(INDEX(C5:C7,$A$4)&lt;&gt;0,INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -3844,13 +3869,13 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
@@ -3965,7 +3990,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -4001,7 +4026,7 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -4115,7 +4140,7 @@
       </c>
       <c r="AD7" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
@@ -4123,7 +4148,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -4131,7 +4156,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="5" t="s">
         <v>77</v>
       </c>
@@ -4139,7 +4164,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="5" t="s">
         <v>79</v>
       </c>
@@ -4147,7 +4172,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="5" t="s">
         <v>81</v>
       </c>
@@ -4155,7 +4180,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="5" t="s">
         <v>83</v>
       </c>
@@ -4163,7 +4188,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="5" t="s">
         <v>85</v>
       </c>
@@ -4171,7 +4196,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
@@ -4179,7 +4204,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="5" t="s">
         <v>89</v>
       </c>
@@ -4187,7 +4212,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="5" t="s">
         <v>91</v>
       </c>
@@ -4195,7 +4220,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="5" t="s">
         <v>93</v>
       </c>
@@ -4203,7 +4228,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="5" t="s">
         <v>95</v>
       </c>
@@ -4211,7 +4236,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="5" t="s">
         <v>97</v>
       </c>
@@ -4219,7 +4244,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="5" t="s">
         <v>99</v>
       </c>
@@ -4227,7 +4252,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="5" t="s">
         <v>101</v>
       </c>
@@ -4235,7 +4260,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="5" t="s">
         <v>103</v>
       </c>
@@ -4243,7 +4268,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="5" t="s">
         <v>105</v>
       </c>
@@ -4251,7 +4276,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="5" t="s">
         <v>107</v>
       </c>
@@ -4259,7 +4284,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="5" t="s">
         <v>109</v>
       </c>
@@ -4267,7 +4292,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="5" t="s">
         <v>111</v>
       </c>
@@ -4275,7 +4300,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="5" t="s">
         <v>113</v>
       </c>
@@ -4283,7 +4308,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="5" t="s">
         <v>115</v>
       </c>
@@ -4291,7 +4316,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="5" t="s">
         <v>117</v>
       </c>
@@ -4299,7 +4324,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="5" t="s">
         <v>119</v>
       </c>
@@ -4307,7 +4332,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="5" t="s">
         <v>121</v>
       </c>
@@ -4315,7 +4340,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="5" t="s">
         <v>123</v>
       </c>
@@ -4323,7 +4348,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="5" t="s">
         <v>125</v>
       </c>
@@ -4331,7 +4356,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>127</v>
       </c>
@@ -4340,56 +4365,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2" r:id="rId3" name="Drop Down 1">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <legacyDrawing r:id="rIdvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:AB39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="7"/>
       <c r="B3" s="11" t="s">
         <v>6</v>
@@ -4400,7 +4397,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="9" t="s">
         <v>12</v>
@@ -4418,25 +4415,25 @@
         <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="L4" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="N4" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="O4" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="Q4" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="R4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>37</v>
@@ -4446,173 +4443,192 @@
         <v>IE</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="K5">
+        <v>165</v>
+      </c>
+      <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>128</v>
-      </c>
-      <c r="N5">
+        <v>159</v>
+      </c>
+      <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q5">
+        <v>163</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="str">
         <f>Regions!D3</f>
         <v>National</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="K6">
+      <c r="E6" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K6" t="n">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6">
+        <v>159</v>
+      </c>
+      <c r="N6" t="n">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q6">
+        <v>164</v>
+      </c>
+      <c r="Q6" t="n">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="str">
         <f>Regions!E3</f>
         <v>IE-CW</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="K7">
+      <c r="G7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="K7" t="n">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>128</v>
-      </c>
-      <c r="N7">
+        <v>160</v>
+      </c>
+      <c r="N7" t="n">
         <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q7">
+        <v>164</v>
+      </c>
+      <c r="Q7" t="n">
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="str">
         <f>Regions!F3</f>
         <v>IE-D</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>162</v>
+      </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="K8">
+      <c r="G8" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K8" t="n">
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>128</v>
-      </c>
-      <c r="N8">
+        <v>160</v>
+      </c>
+      <c r="N8" t="n">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q8">
+        <v>164</v>
+      </c>
+      <c r="Q8" t="n">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="str">
         <f>Regions!G3</f>
         <v>IE-KE</v>
       </c>
-      <c r="K9">
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9" t="s">
+        <v>169</v>
+      </c>
+      <c r="K9" t="n">
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>128</v>
-      </c>
-      <c r="N9">
+        <v>160</v>
+      </c>
+      <c r="N9" t="n">
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q9">
+        <v>164</v>
+      </c>
+      <c r="Q9" t="n">
         <v>4</v>
       </c>
       <c r="R9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="str">
         <f>Regions!H3</f>
         <v>IE-KK</v>
       </c>
-      <c r="K10">
+      <c r="K10" t="n">
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>128</v>
-      </c>
-      <c r="N10">
+        <v>161</v>
+      </c>
+      <c r="N10" t="n">
         <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q10">
+        <v>164</v>
+      </c>
+      <c r="Q10" t="n">
         <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="str">
@@ -4620,26 +4636,26 @@
         <v>IE-LS</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="K11">
+      <c r="K11" t="n">
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>128</v>
-      </c>
-      <c r="N11">
+        <v>161</v>
+      </c>
+      <c r="N11" t="n">
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q11">
+        <v>163</v>
+      </c>
+      <c r="Q11" t="n">
         <v>6</v>
       </c>
       <c r="R11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="str">
@@ -4647,20 +4663,20 @@
         <v>IE-LD</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="K12">
+      <c r="K12" t="n">
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q12">
+        <v>161</v>
+      </c>
+      <c r="Q12" t="n">
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="str">
@@ -4668,20 +4684,20 @@
         <v>IE-LH</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="K13">
+      <c r="K13" t="n">
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q13">
+        <v>162</v>
+      </c>
+      <c r="Q13" t="n">
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="str">
@@ -4689,20 +4705,20 @@
         <v>IE-MH</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="K14">
+      <c r="K14" t="n">
         <v>9</v>
       </c>
       <c r="L14" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q14">
+        <v>162</v>
+      </c>
+      <c r="Q14" t="n">
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="str">
@@ -4710,20 +4726,20 @@
         <v>IE-OY</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="K15">
+      <c r="K15" t="n">
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q15">
+        <v>162</v>
+      </c>
+      <c r="Q15" t="n">
         <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="str">
@@ -4731,20 +4747,20 @@
         <v>IE-WH</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="K16">
+      <c r="K16" t="n">
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q16">
+        <v>159</v>
+      </c>
+      <c r="Q16" t="n">
         <v>11</v>
       </c>
       <c r="R16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="str">
@@ -4752,190 +4768,190 @@
         <v>IE-WX</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="Q17">
+      <c r="Q17" t="n">
         <v>12</v>
       </c>
       <c r="R17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="str">
         <f>Regions!P3</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" t="n">
         <v>13</v>
       </c>
       <c r="R18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="str">
         <f>Regions!Q3</f>
         <v>IE-CE</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" t="n">
         <v>14</v>
       </c>
       <c r="R19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="str">
         <f>Regions!R3</f>
         <v>IE-CO</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" t="n">
         <v>15</v>
       </c>
       <c r="R20" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="str">
         <f>Regions!S3</f>
         <v>IE-KY</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" t="n">
         <v>16</v>
       </c>
       <c r="R21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="str">
         <f>Regions!T3</f>
         <v>IE-LK</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" t="n">
         <v>17</v>
       </c>
       <c r="R22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="str">
         <f>Regions!U3</f>
         <v>IE-TA</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" t="n">
         <v>18</v>
       </c>
       <c r="R23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="str">
         <f>Regions!V3</f>
         <v>IE-WD</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" t="n">
         <v>19</v>
       </c>
       <c r="R24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="str">
         <f>Regions!W3</f>
         <v>IE-G</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" t="n">
         <v>20</v>
       </c>
       <c r="R25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="str">
         <f>Regions!X3</f>
         <v>IE-LM</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" t="n">
         <v>21</v>
       </c>
       <c r="R26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="str">
         <f>Regions!Y3</f>
         <v>IE-MO</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" t="n">
         <v>22</v>
       </c>
       <c r="R27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="7"/>
       <c r="C28" s="8" t="str">
         <f>Regions!Z3</f>
         <v>IE-RN</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" t="n">
         <v>23</v>
       </c>
       <c r="R28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" s="7"/>
       <c r="C29" s="8" t="str">
         <f>Regions!AA3</f>
         <v>IE-SO</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="7"/>
       <c r="C30" s="8" t="str">
         <f>Regions!AB3</f>
         <v>IE-CN</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="7"/>
       <c r="C31" s="8" t="str">
         <f>Regions!AC3</f>
         <v>IE-DL</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="7"/>
       <c r="C32" s="8" t="str">
         <f>Regions!AD3</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="7"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
@@ -4944,19 +4960,19 @@
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" s="7"/>
     </row>
   </sheetData>
@@ -4964,312 +4980,312 @@
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:D45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4">
+    <row r="4">
+      <c r="B4" t="n">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="14" t="s">
         <v>66</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="16" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="13">
+    <row r="13">
+      <c r="B13" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="13">
+    <row r="14">
+      <c r="B14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="13">
+    <row r="15">
+      <c r="B15" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="13">
+    <row r="16">
+      <c r="B16" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="13">
+    <row r="17">
+      <c r="B17" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="13">
+    <row r="18">
+      <c r="B18" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
+    <row r="19">
+      <c r="B19" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
+    <row r="20">
+      <c r="B20" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
+    <row r="21">
+      <c r="B21" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="13">
+    <row r="22">
+      <c r="B22" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="13">
+    <row r="23">
+      <c r="B23" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="13">
+    <row r="24">
+      <c r="B24" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="B25" s="13"/>
-      <c r="C25" s="13">
+      <c r="C25" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="B26" s="13"/>
-      <c r="C26" s="13">
+      <c r="C26" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="B27" s="13"/>
-      <c r="C27" s="13">
+      <c r="C27" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="19">
+    <row r="28">
+      <c r="D28" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="19">
+    <row r="29">
+      <c r="D29" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="19">
+    <row r="30">
+      <c r="D30" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="19">
+    <row r="31">
+      <c r="D31" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="19">
+    <row r="32">
+      <c r="D32" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" s="19">
+    <row r="33">
+      <c r="D33" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" s="19">
+    <row r="34">
+      <c r="D34" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="19">
+    <row r="35">
+      <c r="D35" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" s="19">
+    <row r="36">
+      <c r="D36" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="19">
+    <row r="37">
+      <c r="D37" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" s="19">
+    <row r="38">
+      <c r="D38" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="19">
+    <row r="39">
+      <c r="D39" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="19">
+    <row r="40">
+      <c r="D40" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="19">
+    <row r="41">
+      <c r="D41" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="19">
+    <row r="42">
+      <c r="D42" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D43" s="19">
+    <row r="43">
+      <c r="D43" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D44" s="19">
+    <row r="44">
+      <c r="D44" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D45" s="19">
+    <row r="45">
+      <c r="D45" s="13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5281,68 +5297,68 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B3:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+    <row r="3">
+      <c r="B3" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="17" t="s">
+    <row r="4">
+      <c r="B4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+    <row r="5">
+      <c r="B5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="13" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="B9" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5354,49 +5370,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="24"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -5414,7 +5430,7 @@
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5432,7 +5448,7 @@
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -5450,7 +5466,7 @@
       <c r="O10" s="26"/>
       <c r="P10" s="26"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -5468,7 +5484,7 @@
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -5486,7 +5502,7 @@
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" ht="18.75" customHeight="1">
       <c r="A13" s="20" t="s">
         <v>56</v>
       </c>
@@ -5505,7 +5521,7 @@
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="25" t="s">
         <v>0</v>
       </c>
@@ -5525,7 +5541,7 @@
       <c r="O14" s="26"/>
       <c r="P14" s="26"/>
     </row>
-    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
@@ -5575,7 +5591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26" t="s">
@@ -5583,7 +5599,7 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="26">
+      <c r="F16" s="26" t="n">
         <v>2222</v>
       </c>
       <c r="G16" s="26"/>
@@ -5601,7 +5617,7 @@
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26" t="s">
@@ -5609,7 +5625,7 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="26">
+      <c r="F17" s="26" t="n">
         <v>8888</v>
       </c>
       <c r="G17" s="26"/>
@@ -5627,7 +5643,7 @@
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -5645,7 +5661,7 @@
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -5663,7 +5679,7 @@
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -5681,7 +5697,7 @@
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -5699,7 +5715,7 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -5717,7 +5733,7 @@
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -5735,7 +5751,7 @@
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -5761,34 +5777,34 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="14" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="B1" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" ht="13.5" customHeight="1">
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
@@ -5808,15 +5824,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="7" t="n">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28" t="s">
@@ -5824,11 +5840,11 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
-      <c r="G6" s="28">
+      <c r="G6" s="28" t="n">
         <v>0.04</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
@@ -5841,12 +5857,12 @@
       <c r="F7" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="29" t="n">
         <f>CPI!$D$21/CPI!D3</f>
         <v>1.3926669328933141</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B4,2))</f>
@@ -5859,12 +5875,12 @@
       <c r="F8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="27" t="n">
         <f>CPI!$D$21/CPI!D4</f>
         <v>1.3626878012654737</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B5,2))</f>
@@ -5877,12 +5893,12 @@
       <c r="F9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="27" t="n">
         <f>CPI!$D$21/CPI!D5</f>
         <v>1.3346599424735295</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B6,2))</f>
@@ -5895,12 +5911,12 @@
       <c r="F10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="27" t="n">
         <f>CPI!$D$21/CPI!D6</f>
         <v>1.3084901396799309</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B7,2))</f>
@@ -5913,12 +5929,12 @@
       <c r="F11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="27" t="n">
         <f>CPI!$D$21/CPI!D7</f>
         <v>1.2828334702744419</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B8,2))</f>
@@ -5931,12 +5947,12 @@
       <c r="F12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="27" t="n">
         <f>CPI!$D$21/CPI!D8</f>
         <v>1.2552186597597279</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B9,2))</f>
@@ -5949,12 +5965,12 @@
       <c r="F13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="27" t="n">
         <f>CPI!$D$21/CPI!D9</f>
         <v>1.2281982972208687</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B10,2))</f>
@@ -5967,12 +5983,12 @@
       <c r="F14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="27" t="n">
         <f>CPI!$D$21/CPI!D10</f>
         <v>1.2005848457682002</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B11,2))</f>
@@ -5985,12 +6001,12 @@
       <c r="F15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="27" t="n">
         <f>CPI!$D$21/CPI!D11</f>
         <v>1.1577481637108971</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B12,2))</f>
@@ -6003,12 +6019,12 @@
       <c r="F16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="27" t="n">
         <f>CPI!$D$21/CPI!D12</f>
         <v>1.1462853106048485</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B13,2))</f>
@@ -6021,12 +6037,12 @@
       <c r="F17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="27" t="n">
         <f>CPI!$D$21/CPI!D13</f>
         <v>1.1227084335013209</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B14,2))</f>
@@ -6039,12 +6055,12 @@
       <c r="F18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="27" t="n">
         <f>CPI!$D$21/CPI!D14</f>
         <v>1.0889509539295061</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B15,2))</f>
@@ -6057,12 +6073,12 @@
       <c r="F19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="27" t="n">
         <f>CPI!$D$21/CPI!D15</f>
         <v>1.0613557055843141</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B16,2))</f>
@@ -6075,12 +6091,12 @@
       <c r="F20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="27" t="n">
         <f>CPI!$D$21/CPI!D16</f>
         <v>1.045670645895876</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B17,2))</f>
@@ -6093,12 +6109,12 @@
       <c r="F21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="27" t="n">
         <f>CPI!$D$21/CPI!D17</f>
         <v>1.0394340416460002</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B18,2))</f>
@@ -6111,12 +6127,12 @@
       <c r="F22" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="27" t="n">
         <f>CPI!$D$21/CPI!D18</f>
         <v>1.0383956459999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B19,2))</f>
@@ -6129,12 +6145,12 @@
       <c r="F23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="27" t="n">
         <f>CPI!$D$21/CPI!D19</f>
         <v>1.0363230000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B20,2))</f>
@@ -6147,12 +6163,12 @@
       <c r="F24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="27" t="n">
         <f>CPI!$D$21/CPI!D20</f>
         <v>1.0190000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
         <v>68</v>
@@ -6164,21 +6180,21 @@
       <c r="F25" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="27" t="n">
         <f>CPI!$D$21/CPI!D22</f>
         <v>0.98522167487684731</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="B34" s="27"/>
     </row>
   </sheetData>
@@ -6189,19 +6205,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:P23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
@@ -6212,7 +6228,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" ht="13.5" customHeight="1">
       <c r="B3" s="9" t="s">
         <v>48</v>
       </c>
@@ -6250,7 +6266,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="B4" s="7" t="s">
         <v>67</v>
       </c>
@@ -6275,11 +6291,11 @@
       <c r="O4" t="s">
         <v>63</v>
       </c>
-      <c r="P4">
+      <c r="P4" t="n">
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="B5" s="7" t="str">
         <f>Constants!C7</f>
         <v>EUR00</v>
@@ -6305,11 +6321,11 @@
       <c r="O5" t="s">
         <v>149</v>
       </c>
-      <c r="P5">
+      <c r="P5" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="7" t="str">
         <f>Constants!C8</f>
         <v>EUR01</v>
@@ -6335,11 +6351,11 @@
       <c r="O6" t="s">
         <v>157</v>
       </c>
-      <c r="P6">
+      <c r="P6" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="7" t="str">
         <f>Constants!C9</f>
         <v>EUR02</v>
@@ -6350,11 +6366,11 @@
       <c r="O7" t="s">
         <v>63</v>
       </c>
-      <c r="P7">
+      <c r="P7" t="n">
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="7" t="str">
         <f>Constants!C10</f>
         <v>EUR03</v>
@@ -6365,11 +6381,11 @@
       <c r="O8" t="s">
         <v>63</v>
       </c>
-      <c r="P8">
+      <c r="P8" t="n">
         <v>41.87</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="B9" s="7" t="str">
         <f>Constants!C11</f>
         <v>EUR04</v>
@@ -6380,11 +6396,11 @@
       <c r="O9" t="s">
         <v>63</v>
       </c>
-      <c r="P9">
+      <c r="P9" t="n">
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="B10" s="7" t="str">
         <f>Constants!C12</f>
         <v>EUR05</v>
@@ -6395,11 +6411,11 @@
       <c r="O10" t="s">
         <v>149</v>
       </c>
-      <c r="P10">
+      <c r="P10" t="n">
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="B11" s="7" t="str">
         <f>Constants!C13</f>
         <v>EUR06</v>
@@ -6410,11 +6426,11 @@
       <c r="O11" t="s">
         <v>63</v>
       </c>
-      <c r="P11">
+      <c r="P11" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="7" t="str">
         <f>Constants!C14</f>
         <v>EUR07</v>
@@ -6425,11 +6441,11 @@
       <c r="O12" t="s">
         <v>63</v>
       </c>
-      <c r="P12">
+      <c r="P12" t="n">
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="B13" s="7" t="str">
         <f>Constants!C15</f>
         <v>EUR08</v>
@@ -6440,11 +6456,11 @@
       <c r="O13" t="s">
         <v>63</v>
       </c>
-      <c r="P13">
+      <c r="P13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="B14" s="7" t="str">
         <f>Constants!C16</f>
         <v>EUR09</v>
@@ -6455,11 +6471,11 @@
       <c r="O14" t="s">
         <v>149</v>
       </c>
-      <c r="P14">
+      <c r="P14" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="B15" s="7" t="str">
         <f>Constants!C17</f>
         <v>EUR10</v>
@@ -6470,53 +6486,53 @@
       <c r="O15" t="s">
         <v>157</v>
       </c>
-      <c r="P15">
+      <c r="P15" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="B16" s="7" t="str">
         <f>Constants!C18</f>
         <v>EUR11</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="B17" s="7" t="str">
         <f>Constants!C19</f>
         <v>EUR12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="B18" s="7" t="str">
         <f>Constants!C20</f>
         <v>EUR13</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="B19" s="7" t="str">
         <f>Constants!C21</f>
         <v>EUR14</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="B20" s="7" t="str">
         <f>Constants!C22</f>
         <v>EUR15</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="B21" s="7" t="str">
         <f>Constants!C23</f>
         <v>EUR16</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="B22" s="7" t="str">
         <f>Constants!C24</f>
         <v>EUR17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="B23" s="7" t="str">
         <f>Constants!C25</f>
         <v>EUR19</v>
@@ -6530,20 +6546,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B2:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="30" customHeight="1">
       <c r="B2" s="30"/>
       <c r="C2" s="31" t="s">
         <v>38</v>
@@ -6552,244 +6569,244 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="33">
+    <row r="3" ht="15" customHeight="1">
+      <c r="B3" s="33" t="n">
         <v>2000</v>
       </c>
       <c r="C3" s="34"/>
-      <c r="D3" s="34">
+      <c r="D3" s="34" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="33">
+    <row r="4" ht="15" customHeight="1">
+      <c r="B4" s="33" t="n">
         <v>2001</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="34" t="n">
         <f t="shared" ref="D4:D22" si="0">D3+D3*C4</f>
         <v>102.2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="33">
+    <row r="5" ht="15" customHeight="1">
+      <c r="B5" s="33" t="n">
         <v>2002</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="35" t="n">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="36" t="n">
         <f t="shared" si="0"/>
         <v>104.34620000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="33">
+    <row r="6" ht="15" customHeight="1">
+      <c r="B6" s="33" t="n">
         <v>2003</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="35" t="n">
         <v>0.02</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="36" t="n">
         <f t="shared" si="0"/>
         <v>106.43312400000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="33">
+    <row r="7" ht="15" customHeight="1">
+      <c r="B7" s="33" t="n">
         <v>2004</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="35" t="n">
         <v>0.02</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="36" t="n">
         <f t="shared" si="0"/>
         <v>108.56178648000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="33">
+    <row r="8" ht="15" customHeight="1">
+      <c r="B8" s="33" t="n">
         <v>2005</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="36" t="n">
         <f t="shared" si="0"/>
         <v>110.95014578256001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="33">
+    <row r="9" ht="15" customHeight="1">
+      <c r="B9" s="33" t="n">
         <v>2006</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="35" t="n">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="36" t="n">
         <f t="shared" si="0"/>
         <v>113.39104898977634</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="33">
+    <row r="10" ht="15" customHeight="1">
+      <c r="B10" s="33" t="n">
         <v>2007</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="35" t="n">
         <v>2.3E-2</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="36" t="n">
         <f t="shared" si="0"/>
         <v>115.99904311654119</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="33">
+    <row r="11" ht="15" customHeight="1">
+      <c r="B11" s="33" t="n">
         <v>2008</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="35" t="n">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="36" t="n">
         <f t="shared" si="0"/>
         <v>120.29100771185321</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="33">
+    <row r="12" ht="15" customHeight="1">
+      <c r="B12" s="33" t="n">
         <v>2009</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="35" t="n">
         <v>0.01</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="36" t="n">
         <f t="shared" si="0"/>
         <v>121.49391778897174</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="33">
+    <row r="13" ht="15" customHeight="1">
+      <c r="B13" s="33" t="n">
         <v>2010</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="35" t="n">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="36" t="n">
         <f t="shared" si="0"/>
         <v>124.04529006254015</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="33">
+    <row r="14" ht="15" customHeight="1">
+      <c r="B14" s="33" t="n">
         <v>2011</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="35" t="n">
         <v>3.1E-2</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="36" t="n">
         <f t="shared" si="0"/>
         <v>127.89069405447889</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="33">
+    <row r="15" ht="15" customHeight="1">
+      <c r="B15" s="33" t="n">
         <v>2012</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="35" t="n">
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="36" t="n">
         <f t="shared" si="0"/>
         <v>131.21585209989533</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="33">
+    <row r="16" ht="15" customHeight="1">
+      <c r="B16" s="33" t="n">
         <v>2013</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="35" t="n">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="36" t="n">
         <f t="shared" si="0"/>
         <v>133.18408988139376</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="33">
+    <row r="17" ht="15" customHeight="1">
+      <c r="B17" s="33" t="n">
         <v>2014</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="35" t="n">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="36" t="n">
         <f t="shared" si="0"/>
         <v>133.98319442068211</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="33">
+    <row r="18" ht="15" customHeight="1">
+      <c r="B18" s="33" t="n">
         <v>2015</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="41" t="n">
         <v>1E-3</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="36" t="n">
         <f>D17+D17*C18</f>
         <v>134.1171776151028</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="38">
+    <row r="19" ht="15" customHeight="1">
+      <c r="B19" s="38" t="n">
         <v>2016</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="39" t="n">
         <v>2E-3</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="40" t="n">
         <f t="shared" si="0"/>
         <v>134.385411970333</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="38">
+    <row r="20" ht="15" customHeight="1">
+      <c r="B20" s="38" t="n">
         <v>2017</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="39" t="n">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="40" t="n">
         <f t="shared" si="0"/>
         <v>136.66996397382866</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
+    <row r="21" ht="15" customHeight="1">
+      <c r="B21" s="38" t="n">
         <v>2018</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="39" t="n">
         <v>1.9E-2</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="40" t="n">
         <f t="shared" si="0"/>
         <v>139.26669328933141</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="38">
+    <row r="22" ht="15" customHeight="1">
+      <c r="B22" s="38" t="n">
         <v>2019</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="39" t="n">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="40" t="n">
         <f t="shared" si="0"/>
         <v>141.35569368867138</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" ht="15" customHeight="1">
       <c r="B24" s="37" t="s">
         <v>40</v>
       </c>
@@ -6801,26 +6818,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85124094-EF73-46AF-B3F7-671AC3531E13}">
-  <dimension ref="B3:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="B4" t="s">
         <v>135</v>
       </c>
@@ -6834,7 +6851,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="B5" t="s">
         <v>137</v>
       </c>
@@ -6850,5 +6867,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add a period definition including 2022 as a single year and update cases
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E13076E-08FA-422B-8AF6-6176E8581E6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F8DA62-E4E0-497A-A9CC-0AB1AE82F43F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="160">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -545,6 +545,9 @@
   </si>
   <si>
     <t>P33</t>
+  </si>
+  <si>
+    <t>P13</t>
   </si>
 </sst>
 </file>
@@ -857,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -927,6 +930,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1909,16 +1913,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>402909</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>183834</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1933,8 +1937,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4252913" y="395287"/>
-          <a:ext cx="6927534" cy="1924051"/>
+          <a:off x="6972300" y="319087"/>
+          <a:ext cx="7746684" cy="1905001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4376,8 +4380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AB39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4973,303 +4977,350 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:D45"/>
+  <dimension ref="B3:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="2" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="E12" s="42" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="13">
         <v>1</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="13">
         <v>4</v>
       </c>
       <c r="C14" s="13">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13">
         <v>1</v>
       </c>
-      <c r="D14" s="19">
+      <c r="E14" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="13">
         <v>5</v>
       </c>
       <c r="C15" s="13">
         <v>1</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="13">
         <v>5</v>
       </c>
       <c r="C16" s="13">
+        <v>5</v>
+      </c>
+      <c r="D16" s="13">
         <v>1</v>
       </c>
-      <c r="D16" s="19">
+      <c r="E16" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="13">
         <v>5</v>
       </c>
       <c r="C17" s="13">
+        <v>5</v>
+      </c>
+      <c r="D17" s="13">
         <v>1</v>
       </c>
-      <c r="D17" s="19">
+      <c r="E17" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="13">
         <v>5</v>
       </c>
       <c r="C18" s="13">
         <v>5</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="13">
+        <v>5</v>
+      </c>
+      <c r="E18" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="13">
         <v>5</v>
       </c>
       <c r="C19" s="13">
         <v>5</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="13">
+        <v>5</v>
+      </c>
+      <c r="E19" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="13">
         <v>5</v>
       </c>
       <c r="C20" s="13">
         <v>5</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="13">
+        <v>5</v>
+      </c>
+      <c r="E20" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="13">
         <v>5</v>
       </c>
       <c r="C21" s="13">
         <v>5</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="13">
+        <v>5</v>
+      </c>
+      <c r="E21" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="13">
         <v>5</v>
       </c>
       <c r="C22" s="13">
         <v>5</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="13">
+        <v>5</v>
+      </c>
+      <c r="E22" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="13">
         <v>5</v>
       </c>
       <c r="C23" s="13">
         <v>5</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="13">
+        <v>5</v>
+      </c>
+      <c r="E23" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="13">
         <v>5</v>
       </c>
       <c r="C24" s="13">
         <v>5</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="13">
+        <v>5</v>
+      </c>
+      <c r="E24" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="13"/>
       <c r="C25" s="13">
         <v>5</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="13">
+        <v>5</v>
+      </c>
+      <c r="E25" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="13">
+      <c r="C26" s="13"/>
+      <c r="D26" s="13">
         <v>5</v>
       </c>
-      <c r="D26" s="19">
+      <c r="E26" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="13"/>
-      <c r="C27" s="13">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13">
         <v>5</v>
       </c>
-      <c r="D27" s="19">
+      <c r="E27" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="19">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="19">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="19">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="19">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="19">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" s="19">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" s="19">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="19">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" s="19">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="19">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" s="19">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="19">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="19">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="19">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="19">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D43" s="19">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D44" s="19">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E44" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D45" s="19">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E45" s="19">
         <v>1</v>
       </c>
     </row>
@@ -5764,7 +5815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated time-periods to include P5 and P9 for debugging runs
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F8DA62-E4E0-497A-A9CC-0AB1AE82F43F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46DAE1C-D1CF-4933-88B5-CD892FAC69AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="3900" windowWidth="42165" windowHeight="23985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="162">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -548,6 +548,12 @@
   </si>
   <si>
     <t>P13</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P9</t>
   </si>
 </sst>
 </file>
@@ -860,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -878,7 +884,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -929,7 +934,6 @@
     <xf numFmtId="10" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -4380,7 +4384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -4977,10 +4981,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:E45"/>
+  <dimension ref="B3:G45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4992,49 +4996,55 @@
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="E12" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="G12" s="41" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="13">
         <v>1</v>
       </c>
@@ -5044,290 +5054,327 @@
       <c r="D13" s="13">
         <v>1</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13">
         <v>4</v>
       </c>
-      <c r="C14" s="13">
+      <c r="E14" s="13">
         <v>3</v>
       </c>
-      <c r="D14" s="13">
+      <c r="F14" s="13">
         <v>1</v>
       </c>
-      <c r="E14" s="19">
+      <c r="G14" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15" s="13">
         <v>1</v>
       </c>
       <c r="D15" s="13">
+        <v>5</v>
+      </c>
+      <c r="E15" s="13">
         <v>1</v>
       </c>
-      <c r="E15" s="19">
+      <c r="F15" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G15" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="13">
+        <v>20</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
         <v>5</v>
       </c>
-      <c r="C16" s="13">
+      <c r="E16" s="13">
         <v>5</v>
       </c>
-      <c r="D16" s="13">
+      <c r="F16" s="13">
         <v>1</v>
       </c>
-      <c r="E16" s="19">
+      <c r="G16" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="13">
+        <v>20</v>
+      </c>
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13">
         <v>5</v>
       </c>
-      <c r="C17" s="13">
+      <c r="E17" s="13">
         <v>5</v>
       </c>
-      <c r="D17" s="13">
+      <c r="F17" s="13">
         <v>1</v>
       </c>
-      <c r="E17" s="19">
+      <c r="G17" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="13">
-        <v>5</v>
-      </c>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C18" s="13">
         <v>5</v>
       </c>
       <c r="D18" s="13">
         <v>5</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="13">
+        <v>5</v>
+      </c>
+      <c r="F18" s="13">
+        <v>5</v>
+      </c>
+      <c r="G18" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
-        <v>5</v>
-      </c>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C19" s="13">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D19" s="13">
         <v>5</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="13">
+        <v>5</v>
+      </c>
+      <c r="F19" s="13">
+        <v>5</v>
+      </c>
+      <c r="G19" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
-        <v>5</v>
-      </c>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C20" s="13">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D20" s="13">
         <v>5</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="13">
+        <v>5</v>
+      </c>
+      <c r="F20" s="13">
+        <v>5</v>
+      </c>
+      <c r="G20" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
-        <v>5</v>
-      </c>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C21" s="13">
         <v>5</v>
       </c>
       <c r="D21" s="13">
         <v>5</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="13">
+        <v>5</v>
+      </c>
+      <c r="F21" s="13">
+        <v>5</v>
+      </c>
+      <c r="G21" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="13">
-        <v>5</v>
-      </c>
-      <c r="C22" s="13">
-        <v>5</v>
-      </c>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D22" s="13">
         <v>5</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="13">
+        <v>5</v>
+      </c>
+      <c r="F22" s="13">
+        <v>5</v>
+      </c>
+      <c r="G22" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="13">
-        <v>5</v>
-      </c>
-      <c r="C23" s="13">
-        <v>5</v>
-      </c>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D23" s="13">
         <v>5</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="13">
+        <v>5</v>
+      </c>
+      <c r="F23" s="13">
+        <v>5</v>
+      </c>
+      <c r="G23" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="13">
-        <v>5</v>
-      </c>
-      <c r="C24" s="13">
-        <v>5</v>
-      </c>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D24" s="13">
         <v>5</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="13">
+        <v>5</v>
+      </c>
+      <c r="F24" s="13">
+        <v>5</v>
+      </c>
+      <c r="G24" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E25" s="13">
         <v>5</v>
       </c>
-      <c r="D25" s="13">
+      <c r="F25" s="13">
         <v>5</v>
       </c>
-      <c r="E25" s="19">
+      <c r="G25" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F26" s="13">
         <v>5</v>
       </c>
-      <c r="E26" s="19">
+      <c r="G26" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F27" s="13">
         <v>5</v>
       </c>
-      <c r="E27" s="19">
+      <c r="G27" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E28" s="19">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E29" s="19">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E30" s="19">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E31" s="19">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E32" s="19">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E33" s="19">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E34" s="19">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E35" s="19">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E36" s="19">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E37" s="19">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E38" s="19">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E39" s="19">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E40" s="19">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E41" s="19">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E42" s="19">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E43" s="19">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E44" s="19">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E45" s="19">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="18">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5345,23 +5392,23 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>1</v>
       </c>
     </row>
@@ -5422,387 +5469,387 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
+      <c r="A1" s="23"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="O2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
     </row>
     <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="23" t="s">
+      <c r="N15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="23" t="s">
+      <c r="O15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="23" t="s">
+      <c r="P15" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26">
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25">
         <v>2222</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26">
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25">
         <v>8888</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5830,7 +5877,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>46</v>
       </c>
     </row>
@@ -5868,31 +5915,31 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28">
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27">
         <v>0.04</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="str">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="str">
         <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
         <v>EUR00</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <f>CPI!$D$21/CPI!D3</f>
         <v>1.3926669328933141</v>
       </c>
@@ -5910,7 +5957,7 @@
       <c r="F8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <f>CPI!$D$21/CPI!D4</f>
         <v>1.3626878012654737</v>
       </c>
@@ -5928,7 +5975,7 @@
       <c r="F9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <f>CPI!$D$21/CPI!D5</f>
         <v>1.3346599424735295</v>
       </c>
@@ -5946,7 +5993,7 @@
       <c r="F10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="26">
         <f>CPI!$D$21/CPI!D6</f>
         <v>1.3084901396799309</v>
       </c>
@@ -5964,7 +6011,7 @@
       <c r="F11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="26">
         <f>CPI!$D$21/CPI!D7</f>
         <v>1.2828334702744419</v>
       </c>
@@ -5982,7 +6029,7 @@
       <c r="F12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <f>CPI!$D$21/CPI!D8</f>
         <v>1.2552186597597279</v>
       </c>
@@ -6000,7 +6047,7 @@
       <c r="F13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <f>CPI!$D$21/CPI!D9</f>
         <v>1.2281982972208687</v>
       </c>
@@ -6018,7 +6065,7 @@
       <c r="F14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="26">
         <f>CPI!$D$21/CPI!D10</f>
         <v>1.2005848457682002</v>
       </c>
@@ -6036,7 +6083,7 @@
       <c r="F15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <f>CPI!$D$21/CPI!D11</f>
         <v>1.1577481637108971</v>
       </c>
@@ -6054,7 +6101,7 @@
       <c r="F16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="26">
         <f>CPI!$D$21/CPI!D12</f>
         <v>1.1462853106048485</v>
       </c>
@@ -6072,7 +6119,7 @@
       <c r="F17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="26">
         <f>CPI!$D$21/CPI!D13</f>
         <v>1.1227084335013209</v>
       </c>
@@ -6090,7 +6137,7 @@
       <c r="F18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="26">
         <f>CPI!$D$21/CPI!D14</f>
         <v>1.0889509539295061</v>
       </c>
@@ -6108,7 +6155,7 @@
       <c r="F19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="26">
         <f>CPI!$D$21/CPI!D15</f>
         <v>1.0613557055843141</v>
       </c>
@@ -6126,7 +6173,7 @@
       <c r="F20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="26">
         <f>CPI!$D$21/CPI!D16</f>
         <v>1.045670645895876</v>
       </c>
@@ -6144,7 +6191,7 @@
       <c r="F21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="26">
         <f>CPI!$D$21/CPI!D17</f>
         <v>1.0394340416460002</v>
       </c>
@@ -6162,7 +6209,7 @@
       <c r="F22" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="26">
         <f>CPI!$D$21/CPI!D18</f>
         <v>1.0383956459999999</v>
       </c>
@@ -6180,7 +6227,7 @@
       <c r="F23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="26">
         <f>CPI!$D$21/CPI!D19</f>
         <v>1.0363230000000001</v>
       </c>
@@ -6198,7 +6245,7 @@
       <c r="F24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="26">
         <f>CPI!$D$21/CPI!D20</f>
         <v>1.0190000000000001</v>
       </c>
@@ -6215,7 +6262,7 @@
       <c r="F25" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="26">
         <f>CPI!$D$21/CPI!D22</f>
         <v>0.98522167487684731</v>
       </c>
@@ -6230,7 +6277,7 @@
       <c r="B33" s="7"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
+      <c r="B34" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6595,253 +6642,253 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <v>2000</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="33">
+      <c r="B4" s="32">
         <v>2001</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="34">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="33">
         <f t="shared" ref="D4:D22" si="0">D3+D3*C4</f>
         <v>102.2</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="33">
+      <c r="B5" s="32">
         <v>2002</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="34">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="35">
         <f t="shared" si="0"/>
         <v>104.34620000000001</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="33">
+      <c r="B6" s="32">
         <v>2003</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="34">
         <v>0.02</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="35">
         <f t="shared" si="0"/>
         <v>106.43312400000001</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>2004</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="34">
         <v>0.02</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="35">
         <f t="shared" si="0"/>
         <v>108.56178648000001</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>2005</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="34">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="35">
         <f t="shared" si="0"/>
         <v>110.95014578256001</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>2006</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="34">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="35">
         <f t="shared" si="0"/>
         <v>113.39104898977634</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="33">
+      <c r="B10" s="32">
         <v>2007</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="34">
         <v>2.3E-2</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="35">
         <f t="shared" si="0"/>
         <v>115.99904311654119</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <v>2008</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="34">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="35">
         <f t="shared" si="0"/>
         <v>120.29100771185321</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>2009</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <v>0.01</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="35">
         <f t="shared" si="0"/>
         <v>121.49391778897174</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>2010</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="34">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="35">
         <f t="shared" si="0"/>
         <v>124.04529006254015</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>2011</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="34">
         <v>3.1E-2</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="35">
         <f t="shared" si="0"/>
         <v>127.89069405447889</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="33">
+      <c r="B15" s="32">
         <v>2012</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="34">
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="35">
         <f t="shared" si="0"/>
         <v>131.21585209989533</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="33">
+      <c r="B16" s="32">
         <v>2013</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="34">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="35">
         <f t="shared" si="0"/>
         <v>133.18408988139376</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="33">
+      <c r="B17" s="32">
         <v>2014</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="34">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="35">
         <f t="shared" si="0"/>
         <v>133.98319442068211</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>2015</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="40">
         <v>1E-3</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="35">
         <f>D17+D17*C18</f>
         <v>134.1171776151028</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="38">
+      <c r="B19" s="37">
         <v>2016</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="38">
         <v>2E-3</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="39">
         <f t="shared" si="0"/>
         <v>134.385411970333</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="38">
+      <c r="B20" s="37">
         <v>2017</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="38">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="39">
         <f t="shared" si="0"/>
         <v>136.66996397382866</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
+      <c r="B21" s="37">
         <v>2018</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="38">
         <v>1.9E-2</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="39">
         <f t="shared" si="0"/>
         <v>139.26669328933141</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="38">
+      <c r="B22" s="37">
         <v>2019</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="39">
         <f t="shared" si="0"/>
         <v>141.35569368867138</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add additional period definitions
- yearly until 2032 followed by 5 year steps (P23)
- as above, except starting with 2 years (P22)
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46DAE1C-D1CF-4933-88B5-CD892FAC69AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A523D86D-04D8-4B15-9A19-376FF8D73A5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="3900" windowWidth="42165" windowHeight="23985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="164">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -554,6 +554,12 @@
   </si>
   <si>
     <t>P9</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>P23</t>
   </si>
 </sst>
 </file>
@@ -1917,13 +1923,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>183834</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
@@ -4981,50 +4987,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:G45"/>
+  <dimension ref="B3:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="2" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
         <v>160</v>
       </c>
@@ -5041,10 +5044,16 @@
         <v>41</v>
       </c>
       <c r="G12" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" s="41" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="13">
         <v>1</v>
       </c>
@@ -5060,11 +5069,17 @@
       <c r="F13" s="13">
         <v>1</v>
       </c>
-      <c r="G13" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="13">
         <v>1</v>
       </c>
@@ -5080,11 +5095,17 @@
       <c r="F14" s="13">
         <v>1</v>
       </c>
-      <c r="G14" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="13">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1</v>
+      </c>
+      <c r="I14" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="13">
         <v>1</v>
       </c>
@@ -5100,11 +5121,17 @@
       <c r="F15" s="13">
         <v>1</v>
       </c>
-      <c r="G15" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="13">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1</v>
+      </c>
+      <c r="I15" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="13">
         <v>20</v>
       </c>
@@ -5120,11 +5147,17 @@
       <c r="F16" s="13">
         <v>1</v>
       </c>
-      <c r="G16" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="13">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1</v>
+      </c>
+      <c r="I16" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="13">
         <v>20</v>
       </c>
@@ -5140,11 +5173,17 @@
       <c r="F17" s="13">
         <v>1</v>
       </c>
-      <c r="G17" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="13">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1</v>
+      </c>
+      <c r="I17" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="13">
         <v>5</v>
       </c>
@@ -5157,11 +5196,17 @@
       <c r="F18" s="13">
         <v>5</v>
       </c>
-      <c r="G18" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="13">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13">
+        <v>1</v>
+      </c>
+      <c r="I18" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C19" s="13">
         <v>45</v>
       </c>
@@ -5174,11 +5219,17 @@
       <c r="F19" s="13">
         <v>5</v>
       </c>
-      <c r="G19" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="13">
+        <v>1</v>
+      </c>
+      <c r="H19" s="13">
+        <v>1</v>
+      </c>
+      <c r="I19" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C20" s="13">
         <v>25</v>
       </c>
@@ -5191,11 +5242,17 @@
       <c r="F20" s="13">
         <v>5</v>
       </c>
-      <c r="G20" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="13">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13">
+        <v>1</v>
+      </c>
+      <c r="I20" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C21" s="13">
         <v>5</v>
       </c>
@@ -5208,11 +5265,17 @@
       <c r="F21" s="13">
         <v>5</v>
       </c>
-      <c r="G21" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>1</v>
+      </c>
+      <c r="I21" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D22" s="13">
         <v>5</v>
       </c>
@@ -5222,11 +5285,17 @@
       <c r="F22" s="13">
         <v>5</v>
       </c>
-      <c r="G22" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="13">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13">
+        <v>1</v>
+      </c>
+      <c r="I22" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D23" s="13">
         <v>5</v>
       </c>
@@ -5236,11 +5305,17 @@
       <c r="F23" s="13">
         <v>5</v>
       </c>
-      <c r="G23" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="13">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
+      <c r="I23" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D24" s="13">
         <v>5</v>
       </c>
@@ -5250,124 +5325,193 @@
       <c r="F24" s="13">
         <v>5</v>
       </c>
-      <c r="G24" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="13">
+        <v>1</v>
+      </c>
+      <c r="H24" s="13">
+        <v>1</v>
+      </c>
+      <c r="I24" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E25" s="13">
         <v>5</v>
       </c>
       <c r="F25" s="13">
         <v>5</v>
       </c>
-      <c r="G25" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="13">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1</v>
+      </c>
+      <c r="I25" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F26" s="13">
         <v>5</v>
       </c>
-      <c r="G26" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="13">
+        <v>1</v>
+      </c>
+      <c r="H26" s="13">
+        <v>1</v>
+      </c>
+      <c r="I26" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F27" s="13">
         <v>5</v>
       </c>
-      <c r="G27" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G28" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G29" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G30" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G31" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G32" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G33" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G34" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G35" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G36" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G37" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G38" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G39" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G40" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G45" s="18">
+      <c r="G27" s="13">
+        <v>5</v>
+      </c>
+      <c r="H27" s="13">
+        <v>1</v>
+      </c>
+      <c r="I27" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G28" s="13">
+        <v>5</v>
+      </c>
+      <c r="H28" s="13">
+        <v>5</v>
+      </c>
+      <c r="I28" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G29" s="13">
+        <v>5</v>
+      </c>
+      <c r="H29" s="13">
+        <v>5</v>
+      </c>
+      <c r="I29" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G30" s="13">
+        <v>5</v>
+      </c>
+      <c r="H30" s="13">
+        <v>5</v>
+      </c>
+      <c r="I30" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G31" s="13">
+        <v>5</v>
+      </c>
+      <c r="H31" s="13">
+        <v>5</v>
+      </c>
+      <c r="I31" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G32" s="13">
+        <v>5</v>
+      </c>
+      <c r="H32" s="13">
+        <v>5</v>
+      </c>
+      <c r="I32" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G33" s="13">
+        <v>5</v>
+      </c>
+      <c r="H33" s="13">
+        <v>5</v>
+      </c>
+      <c r="I33" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G34" s="13">
+        <v>5</v>
+      </c>
+      <c r="H34" s="13">
+        <v>5</v>
+      </c>
+      <c r="I34" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H35" s="13">
+        <v>5</v>
+      </c>
+      <c r="I35" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I45" s="18">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the defunits table
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527E3A4-E962-433B-AEA6-03868971AB01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB5F11F-8ED4-40E4-9029-29D8FABD08E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10710" yWindow="2670" windowWidth="15390" windowHeight="9585" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -232,19 +232,10 @@
     <t>IND</t>
   </si>
   <si>
-    <t>ELC</t>
-  </si>
-  <si>
-    <t>COM</t>
-  </si>
-  <si>
     <t>RSD</t>
   </si>
   <si>
     <t>PJ</t>
-  </si>
-  <si>
-    <t>PJ-a</t>
   </si>
   <si>
     <t>GW</t>
@@ -563,6 +554,15 @@
   </si>
   <si>
     <t>EUR20</t>
+  </si>
+  <si>
+    <t>Pja</t>
+  </si>
+  <si>
+    <t>SRV</t>
+  </si>
+  <si>
+    <t>PWR</t>
   </si>
 </sst>
 </file>
@@ -3869,13 +3869,13 @@
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="str">
         <f>A11</f>
@@ -3984,7 +3984,7 @@
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>C5</f>
@@ -4020,7 +4020,7 @@
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" ref="C7:AC7" si="0">D5</f>
@@ -4134,223 +4134,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4435,22 +4435,22 @@
         <v>11</v>
       </c>
       <c r="K4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" t="s">
+        <v>127</v>
+      </c>
+      <c r="N4" t="s">
+        <v>128</v>
+      </c>
+      <c r="O4" t="s">
         <v>129</v>
       </c>
-      <c r="L4" t="s">
+      <c r="Q4" t="s">
         <v>130</v>
       </c>
-      <c r="N4" t="s">
-        <v>131</v>
-      </c>
-      <c r="O4" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>133</v>
-      </c>
       <c r="R4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -4463,31 +4463,31 @@
         <v>IE</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -4504,19 +4504,19 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -4533,19 +4533,19 @@
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q7">
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -4562,19 +4562,19 @@
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q8">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -4588,19 +4588,19 @@
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q9">
         <v>4</v>
       </c>
       <c r="R9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -4614,19 +4614,19 @@
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q10">
         <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -4641,19 +4641,19 @@
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q11">
         <v>6</v>
       </c>
       <c r="R11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -4668,13 +4668,13 @@
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q12">
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -4689,13 +4689,13 @@
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q13">
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -4710,13 +4710,13 @@
         <v>9</v>
       </c>
       <c r="L14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q14">
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -4731,13 +4731,13 @@
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q15">
         <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -4752,13 +4752,13 @@
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q16">
         <v>11</v>
       </c>
       <c r="R16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -4773,7 +4773,7 @@
         <v>12</v>
       </c>
       <c r="R17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -4787,7 +4787,7 @@
         <v>13</v>
       </c>
       <c r="R18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -4801,7 +4801,7 @@
         <v>14</v>
       </c>
       <c r="R19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -4814,7 +4814,7 @@
         <v>15</v>
       </c>
       <c r="R20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -4827,7 +4827,7 @@
         <v>16</v>
       </c>
       <c r="R21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -4840,7 +4840,7 @@
         <v>17</v>
       </c>
       <c r="R22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -4853,7 +4853,7 @@
         <v>18</v>
       </c>
       <c r="R23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -4866,7 +4866,7 @@
         <v>19</v>
       </c>
       <c r="R24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
@@ -4879,7 +4879,7 @@
         <v>20</v>
       </c>
       <c r="R25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -4892,7 +4892,7 @@
         <v>21</v>
       </c>
       <c r="R26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
@@ -4905,7 +4905,7 @@
         <v>22</v>
       </c>
       <c r="R27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -4918,7 +4918,7 @@
         <v>23</v>
       </c>
       <c r="R28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -5032,28 +5032,28 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>41</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
@@ -6084,7 +6084,7 @@
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G7" s="28">
         <f>CPI!$D$21/CPI!D3</f>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G8" s="26">
         <f>CPI!$D$21/CPI!D4</f>
@@ -6120,7 +6120,7 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G9" s="26">
         <f>CPI!$D$21/CPI!D5</f>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G10" s="26">
         <f>CPI!$D$21/CPI!D6</f>
@@ -6156,7 +6156,7 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G11" s="26">
         <f>CPI!$D$21/CPI!D7</f>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G12" s="26">
         <f>CPI!$D$21/CPI!D8</f>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G13" s="26">
         <f>CPI!$D$21/CPI!D9</f>
@@ -6210,7 +6210,7 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G14" s="26">
         <f>CPI!$D$21/CPI!D10</f>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G15" s="26">
         <f>CPI!$D$21/CPI!D11</f>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G16" s="26">
         <f>CPI!$D$21/CPI!D12</f>
@@ -6264,7 +6264,7 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G17" s="26">
         <f>CPI!$D$21/CPI!D13</f>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G18" s="26">
         <f>CPI!$D$21/CPI!D14</f>
@@ -6300,7 +6300,7 @@
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G19" s="26">
         <f>CPI!$D$21/CPI!D15</f>
@@ -6318,7 +6318,7 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G20" s="26">
         <f>CPI!$D$21/CPI!D16</f>
@@ -6336,7 +6336,7 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G21" s="26">
         <f>CPI!$D$21/CPI!D17</f>
@@ -6354,7 +6354,7 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G22" s="26">
         <f>CPI!$D$21/CPI!D18</f>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G23" s="26">
         <f>CPI!$D$21/CPI!D19</f>
@@ -6390,7 +6390,7 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G24" s="26">
         <f>CPI!$D$21/CPI!D20</f>
@@ -6400,14 +6400,14 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G25" s="26">
         <f>CPI!$D$21/CPI!D22</f>
@@ -6416,14 +6416,14 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C26" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G26" s="26">
         <f>CPI!$D$21/CPI!D23</f>
@@ -6454,7 +6454,7 @@
   <dimension ref="B2:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6467,10 +6467,10 @@
         <v>47</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6490,51 +6490,51 @@
         <v>59</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>60</v>
+        <v>164</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>49</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>50</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P4">
         <v>3.6</v>
@@ -6549,22 +6549,22 @@
         <v>51</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="O5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P5">
         <v>1000</v>
@@ -6579,22 +6579,22 @@
         <v>52</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="O6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P6">
         <v>1000</v>
@@ -6606,10 +6606,10 @@
         <v>EUR02</v>
       </c>
       <c r="N7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="O7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P7">
         <v>0.04</v>
@@ -6621,10 +6621,10 @@
         <v>EUR03</v>
       </c>
       <c r="N8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="O8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P8">
         <v>41.87</v>
@@ -6636,10 +6636,10 @@
         <v>EUR04</v>
       </c>
       <c r="N9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="O9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P9">
         <v>3.5999999999999999E-3</v>
@@ -6651,10 +6651,10 @@
         <v>EUR05</v>
       </c>
       <c r="N10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P10">
         <v>1000000</v>
@@ -6666,10 +6666,10 @@
         <v>EUR06</v>
       </c>
       <c r="N11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P11">
         <v>1000</v>
@@ -6681,10 +6681,10 @@
         <v>EUR07</v>
       </c>
       <c r="N12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="O12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P12">
         <v>3.6</v>
@@ -6696,10 +6696,10 @@
         <v>EUR08</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P13">
         <v>1</v>
@@ -6711,10 +6711,10 @@
         <v>EUR09</v>
       </c>
       <c r="N14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="O14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P14">
         <v>1</v>
@@ -6726,10 +6726,10 @@
         <v>EUR10</v>
       </c>
       <c r="N15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P15">
         <v>1</v>
@@ -7096,35 +7096,35 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" t="s">
         <v>138</v>
-      </c>
-      <c r="D5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a period definition with 35 annual periods followed by 4 5-year periods
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2557D1-E129-497E-A1DE-405C4E14DC21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE954B48-2129-4985-9FEB-4A5BBBCF7FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="1800" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="176">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t>SRV</t>
+  </si>
+  <si>
+    <t>P39</t>
   </si>
 </sst>
 </file>
@@ -5132,10 +5135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:I45"/>
+  <dimension ref="B3:J51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5145,34 +5148,34 @@
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
         <v>167</v>
       </c>
@@ -5197,8 +5200,11 @@
       <c r="I12" s="16" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="42">
         <v>1</v>
       </c>
@@ -5223,8 +5229,11 @@
       <c r="I13" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="42">
         <v>1</v>
       </c>
@@ -5249,8 +5258,11 @@
       <c r="I14" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="42">
         <v>1</v>
       </c>
@@ -5275,8 +5287,11 @@
       <c r="I15" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="42">
         <v>20</v>
       </c>
@@ -5301,8 +5316,11 @@
       <c r="I16" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="42">
         <v>20</v>
       </c>
@@ -5327,8 +5345,11 @@
       <c r="I17" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C18" s="42">
         <v>5</v>
       </c>
@@ -5350,8 +5371,11 @@
       <c r="I18" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C19" s="42">
         <v>45</v>
       </c>
@@ -5373,8 +5397,11 @@
       <c r="I19" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C20" s="42">
         <v>25</v>
       </c>
@@ -5396,8 +5423,11 @@
       <c r="I20" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C21" s="42">
         <v>5</v>
       </c>
@@ -5419,8 +5449,11 @@
       <c r="I21" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D22" s="13">
         <v>5</v>
       </c>
@@ -5439,8 +5472,11 @@
       <c r="I22" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D23" s="13">
         <v>5</v>
       </c>
@@ -5459,8 +5495,11 @@
       <c r="I23" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D24" s="13">
         <v>5</v>
       </c>
@@ -5479,8 +5518,11 @@
       <c r="I24" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E25" s="13">
         <v>5</v>
       </c>
@@ -5496,8 +5538,11 @@
       <c r="I25" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="F26" s="13">
         <v>5</v>
       </c>
@@ -5510,8 +5555,11 @@
       <c r="I26" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="F27" s="13">
         <v>5</v>
       </c>
@@ -5524,8 +5572,11 @@
       <c r="I27" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G28" s="42">
         <v>5</v>
       </c>
@@ -5535,8 +5586,11 @@
       <c r="I28" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G29" s="42">
         <v>5</v>
       </c>
@@ -5546,8 +5600,11 @@
       <c r="I29" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G30" s="42">
         <v>5</v>
       </c>
@@ -5557,8 +5614,11 @@
       <c r="I30" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G31" s="42">
         <v>5</v>
       </c>
@@ -5568,8 +5628,11 @@
       <c r="I31" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G32" s="42">
         <v>5</v>
       </c>
@@ -5579,8 +5642,11 @@
       <c r="I32" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G33" s="42">
         <v>5</v>
       </c>
@@ -5590,8 +5656,11 @@
       <c r="I33" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G34" s="42">
         <v>5</v>
       </c>
@@ -5601,63 +5670,129 @@
       <c r="I34" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
       <c r="H35" s="42">
         <v>5</v>
       </c>
       <c r="I35" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I36" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I37" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I38" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I39" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I40" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I41" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I42" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I43" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I44" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="J44" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.2">
       <c r="I45" s="13">
         <v>1</v>
+      </c>
+      <c r="J45" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="J46" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="J47" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="J48" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J49" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J50" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J51" s="13">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6595,7 +6730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bring 40 ts back
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB90EFC2-176E-4AC9-80FC-955A662CAB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843CCBE7-A501-4491-B326-923984028127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="27" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="167">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -450,9 +450,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Season</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -541,6 +538,36 @@
   </si>
   <si>
     <t>PJa</t>
+  </si>
+  <si>
+    <t>Wi</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>Sp</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Au</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -550,7 +577,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -674,6 +701,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -853,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,6 +954,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3338,30 +3373,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="season_info" displayName="season_info" ref="K4:L16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90224694-EE63-4ABC-9297-AB63CB1A1D7F}" name="season_info2" displayName="season_info2" ref="K4:L16" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Month"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Season"/>
+    <tableColumn id="1" xr3:uid="{B98A10FD-44F7-4E1C-B697-1F9915227BC8}" name="Month"/>
+    <tableColumn id="2" xr3:uid="{9B83B8C3-97CC-4A62-8C08-B1F0D8EBB938}" name="Season"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="weekly_info" displayName="weekly_info" ref="N4:O11" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2CF4CA5A-253E-433A-85B9-AFDEA52AACAB}" name="weekly_info3" displayName="weekly_info3" ref="N4:O11" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Day"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Type"/>
+    <tableColumn id="1" xr3:uid="{A228BFBE-A872-426A-B0A9-3C4C603AD3CB}" name="Day"/>
+    <tableColumn id="2" xr3:uid="{0BC14070-CF92-42D1-BB24-90E18C8E60C8}" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="daynite_info" displayName="daynite_info" ref="Q4:R28" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7EF17D7E-DA73-4612-9062-3728FB92AD1D}" name="daynite_info7" displayName="daynite_info7" ref="Q4:R28" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Hour"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
+    <tableColumn id="1" xr3:uid="{15A4E9E6-6EB3-4E8B-A64D-9992514AAFEA}" name="Hour"/>
+    <tableColumn id="2" xr3:uid="{9BA2D8D9-7EE1-486A-9C49-105AADE759D5}" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4371,8 +4406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AB39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4416,19 +4451,19 @@
         <v>126</v>
       </c>
       <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" t="s">
         <v>127</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>128</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>129</v>
       </c>
-      <c r="Q4" t="s">
-        <v>130</v>
-      </c>
       <c r="R4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -4440,26 +4475,26 @@
         <f>Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="42" t="s">
         <v>125</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -4475,20 +4510,26 @@
         <f>Regions!D3</f>
         <v>National</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="E6" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>161</v>
+      </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -4504,20 +4545,24 @@
         <f>Regions!E3</f>
         <v>IE-CW</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="E7" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42" t="s">
+        <v>163</v>
+      </c>
       <c r="K7">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="Q7">
         <v>2</v>
@@ -4533,20 +4578,24 @@
         <f>Regions!F3</f>
         <v>IE-D</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="E8" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42" t="s">
+        <v>165</v>
+      </c>
       <c r="K8">
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="Q8">
         <v>3</v>
@@ -4562,17 +4611,20 @@
         <f>Regions!G3</f>
         <v>IE-KE</v>
       </c>
+      <c r="G9" t="s">
+        <v>166</v>
+      </c>
       <c r="K9">
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="Q9">
         <v>4</v>
@@ -4592,13 +4644,13 @@
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="Q10">
         <v>5</v>
@@ -4619,13 +4671,13 @@
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="Q11">
         <v>6</v>
@@ -4646,13 +4698,13 @@
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="Q12">
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -4667,13 +4719,13 @@
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="Q13">
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -4688,13 +4740,13 @@
         <v>9</v>
       </c>
       <c r="L14" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="Q14">
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -4709,13 +4761,13 @@
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="Q15">
         <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -4730,13 +4782,13 @@
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="Q16">
         <v>11</v>
       </c>
       <c r="R16" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -4751,7 +4803,7 @@
         <v>12</v>
       </c>
       <c r="R17" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -4765,7 +4817,7 @@
         <v>13</v>
       </c>
       <c r="R18" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -4779,7 +4831,7 @@
         <v>14</v>
       </c>
       <c r="R19" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -4792,7 +4844,7 @@
         <v>15</v>
       </c>
       <c r="R20" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -4805,7 +4857,7 @@
         <v>16</v>
       </c>
       <c r="R21" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -4818,7 +4870,7 @@
         <v>17</v>
       </c>
       <c r="R22" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -4831,7 +4883,7 @@
         <v>18</v>
       </c>
       <c r="R23" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -4844,7 +4896,7 @@
         <v>19</v>
       </c>
       <c r="R24" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
@@ -4857,7 +4909,7 @@
         <v>20</v>
       </c>
       <c r="R25" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -4870,7 +4922,7 @@
         <v>21</v>
       </c>
       <c r="R26" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
@@ -4883,7 +4935,7 @@
         <v>22</v>
       </c>
       <c r="R27" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -4896,7 +4948,7 @@
         <v>23</v>
       </c>
       <c r="R28" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -5009,31 +5061,31 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>150</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>41</v>
       </c>
       <c r="G12" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="H12" s="41" t="s">
-        <v>152</v>
-      </c>
       <c r="I12" s="41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J12" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -6525,7 +6577,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C26" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>45</v>
@@ -6576,10 +6628,10 @@
         <v>47</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6599,25 +6651,25 @@
         <v>59</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>49</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>60</v>
       </c>
       <c r="M3" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
@@ -6640,7 +6692,7 @@
         <v>61</v>
       </c>
       <c r="M4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N4" t="s">
         <v>61</v>
@@ -6658,10 +6710,10 @@
         <v>51</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>62</v>
@@ -6670,10 +6722,10 @@
         <v>62</v>
       </c>
       <c r="M5" t="s">
+        <v>136</v>
+      </c>
+      <c r="N5" t="s">
         <v>137</v>
-      </c>
-      <c r="N5" t="s">
-        <v>138</v>
       </c>
       <c r="O5">
         <v>1000</v>
@@ -6700,10 +6752,10 @@
         <v>61</v>
       </c>
       <c r="M6" t="s">
+        <v>144</v>
+      </c>
+      <c r="N6" t="s">
         <v>145</v>
-      </c>
-      <c r="N6" t="s">
-        <v>146</v>
       </c>
       <c r="O6">
         <v>1000</v>
@@ -6715,7 +6767,7 @@
         <v>EUR02</v>
       </c>
       <c r="M7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N7" t="s">
         <v>61</v>
@@ -6730,7 +6782,7 @@
         <v>EUR03</v>
       </c>
       <c r="M8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N8" t="s">
         <v>61</v>
@@ -6745,7 +6797,7 @@
         <v>EUR04</v>
       </c>
       <c r="M9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N9" t="s">
         <v>61</v>
@@ -6760,10 +6812,10 @@
         <v>EUR05</v>
       </c>
       <c r="M10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O10">
         <v>1000000</v>
@@ -6775,7 +6827,7 @@
         <v>EUR06</v>
       </c>
       <c r="M11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N11" t="s">
         <v>61</v>
@@ -6790,7 +6842,7 @@
         <v>EUR07</v>
       </c>
       <c r="M12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N12" t="s">
         <v>61</v>
@@ -6820,10 +6872,10 @@
         <v>EUR09</v>
       </c>
       <c r="M14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -6835,10 +6887,10 @@
         <v>EUR10</v>
       </c>
       <c r="M15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -6909,7 +6961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>